<commit_message>
Cleaned up script naming and removed superfluous files
</commit_message>
<xml_diff>
--- a/inputs/template_input.xlsx
+++ b/inputs/template_input.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\inputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="20736" windowHeight="11760" tabRatio="961"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Causes of death" sheetId="4" r:id="rId3"/>
     <sheet name="Nutritional status distribution" sheetId="5" r:id="rId4"/>
     <sheet name="Breastfeeding distribution" sheetId="50" r:id="rId5"/>
-    <sheet name="Time trends" sheetId="51" state="hidden" r:id="rId6"/>
+    <sheet name="Time trends" sheetId="51" r:id="rId6"/>
     <sheet name="IYCF packages" sheetId="55" r:id="rId7"/>
     <sheet name="Treatment of SAM" sheetId="60" r:id="rId8"/>
     <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
@@ -90,7 +85,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -100,7 +95,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +183,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +241,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -280,7 +275,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +334,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1192,12 +1187,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1492,7 +1487,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2932,7 +2927,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2968,8 +2963,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2979,7 +2974,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2989,16 +2984,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -3031,7 +3026,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3047,8 +3042,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="5" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="19" fillId="3" borderId="5" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3072,7 +3067,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3093,40 +3088,40 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="3" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="5" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3259,7 +3254,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4773,7 +4768,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4830,7 +4825,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4887,7 +4882,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4944,7 +4939,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5001,7 +4996,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5058,7 +5053,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5115,7 +5110,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5172,7 +5167,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5229,7 +5224,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5286,7 +5281,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5343,7 +5338,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5400,7 +5395,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5457,7 +5452,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5514,7 +5509,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5571,7 +5566,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5628,7 +5623,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5685,7 +5680,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5742,7 +5737,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5791,7 +5786,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6160,18 +6155,18 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="14.44140625" style="12"/>
+    <col min="1" max="1" width="27.6328125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6328125" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="14.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -6182,14 +6177,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>193</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>195</v>
@@ -6198,7 +6193,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>194</v>
@@ -6207,7 +6202,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -6262,7 +6257,7 @@
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
@@ -6369,7 +6364,7 @@
       </c>
       <c r="C32" s="69"/>
     </row>
-    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
         <v>129</v>
       </c>
@@ -6379,7 +6374,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
@@ -6532,7 +6527,7 @@
       </c>
       <c r="C59" s="66"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -6556,15 +6551,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="35"/>
+    <col min="2" max="2" width="47.81640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
         <v>189</v>
       </c>
@@ -6584,7 +6579,7 @@
       </c>
       <c r="C2" s="81"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
         <v>206</v>
       </c>
@@ -6593,7 +6588,7 @@
       </c>
       <c r="C3" s="81"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
         <v>58</v>
       </c>
@@ -6602,7 +6597,7 @@
       </c>
       <c r="C4" s="81"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>137</v>
       </c>
@@ -6611,104 +6606,104 @@
       </c>
       <c r="C5" s="81"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
       <c r="B6" s="87"/>
       <c r="C6" s="87"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
       <c r="B7" s="87"/>
       <c r="C7" s="87"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="90"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="90"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="90"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="90"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="90"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="90"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="90"/>
       <c r="B17" s="87"/>
       <c r="C17" s="87"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="90"/>
       <c r="B18" s="87"/>
       <c r="C18" s="87"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="89"/>
       <c r="B19" s="87"/>
       <c r="C19" s="87"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="89"/>
       <c r="B20" s="87"/>
       <c r="C20" s="87"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="89"/>
       <c r="B21" s="87"/>
       <c r="C21" s="87"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="89"/>
       <c r="B22" s="87"/>
       <c r="C22" s="87"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B23" s="87"/>
       <c r="C23" s="87"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B24" s="87"/>
       <c r="C24" s="87"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B25" s="87"/>
       <c r="C25" s="87"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B26" s="87"/>
       <c r="C26" s="87"/>
     </row>
@@ -6731,85 +6726,85 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="35"/>
+    <col min="1" max="1" width="30.08984375" style="35" customWidth="1"/>
+    <col min="2" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="48"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
     </row>
   </sheetData>
@@ -6829,7 +6824,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -6943,19 +6938,19 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -7002,7 +6997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -7517,7 +7512,7 @@
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -7568,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>86</v>
@@ -7613,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>189</v>
@@ -7662,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>206</v>
@@ -7898,7 +7893,7 @@
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="60" t="s">
         <v>37</v>
       </c>
@@ -8148,7 +8143,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -8662,20 +8657,20 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.90625" style="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" style="56" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="56" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.109375" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.33203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="16.109375" style="56"/>
+    <col min="6" max="7" width="13.08984375" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.36328125" style="56" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.90625" style="56" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.08984375" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
         <v>33</v>
       </c>
@@ -8722,7 +8717,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>31</v>
       </c>
@@ -8769,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="53" t="s">
         <v>149</v>
       </c>
@@ -8813,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="53" t="s">
         <v>175</v>
       </c>
@@ -8857,7 +8852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="53" t="s">
         <v>174</v>
       </c>
@@ -8901,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="53" t="s">
         <v>173</v>
       </c>
@@ -8945,7 +8940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="53" t="s">
         <v>196</v>
       </c>
@@ -8989,7 +8984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="53" t="s">
         <v>136</v>
       </c>
@@ -9033,7 +9028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="53" t="s">
         <v>137</v>
       </c>
@@ -9077,7 +9072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="53" t="s">
         <v>84</v>
       </c>
@@ -9121,7 +9116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="53" t="s">
         <v>58</v>
       </c>
@@ -9165,7 +9160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="53" t="s">
         <v>67</v>
       </c>
@@ -9209,7 +9204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="53" t="s">
         <v>28</v>
       </c>
@@ -9253,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="53" t="s">
         <v>85</v>
       </c>
@@ -9297,7 +9292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="53" t="s">
         <v>60</v>
       </c>
@@ -9341,7 +9336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="53"/>
       <c r="C16" s="97"/>
       <c r="D16" s="97"/>
@@ -9357,7 +9352,7 @@
       <c r="N16" s="97"/>
       <c r="O16" s="97"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="57" t="s">
         <v>32</v>
       </c>
@@ -9404,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="57"/>
       <c r="B18" s="53" t="s">
         <v>86</v>
@@ -9449,7 +9444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="98" t="s">
         <v>189</v>
       </c>
@@ -9493,7 +9488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="98" t="s">
         <v>206</v>
       </c>
@@ -9537,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="99" t="s">
         <v>57</v>
       </c>
@@ -9581,7 +9576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="53" t="s">
         <v>88</v>
       </c>
@@ -9625,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="53" t="s">
         <v>87</v>
       </c>
@@ -9669,7 +9664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="53" t="s">
         <v>59</v>
       </c>
@@ -9713,7 +9708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="53"/>
       <c r="C25" s="97"/>
       <c r="D25" s="97"/>
@@ -9729,7 +9724,7 @@
       <c r="N25" s="97"/>
       <c r="O25" s="97"/>
     </row>
-    <row r="26" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="57" t="s">
         <v>37</v>
       </c>
@@ -9777,7 +9772,7 @@
       </c>
       <c r="P26" s="100"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="61" t="s">
         <v>190</v>
       </c>
@@ -9821,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="57"/>
       <c r="B28" s="61" t="s">
         <v>207</v>
@@ -9866,7 +9861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="61" t="s">
         <v>191</v>
       </c>
@@ -9910,7 +9905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="61" t="s">
         <v>192</v>
       </c>
@@ -9954,7 +9949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="53"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -9970,7 +9965,7 @@
       <c r="N31" s="97"/>
       <c r="O31" s="97"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="57" t="s">
         <v>35</v>
       </c>
@@ -10017,7 +10012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="53" t="s">
         <v>64</v>
       </c>
@@ -10061,7 +10056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="53" t="s">
         <v>62</v>
       </c>
@@ -10105,7 +10100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="53" t="s">
         <v>47</v>
       </c>
@@ -10149,7 +10144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="53" t="s">
         <v>34</v>
       </c>
@@ -10193,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="103"/>
       <c r="B37" s="53" t="s">
         <v>83</v>
@@ -10238,7 +10233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="53" t="s">
         <v>82</v>
       </c>
@@ -10282,7 +10277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="53" t="s">
         <v>81</v>
       </c>
@@ -10326,7 +10321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="53" t="s">
         <v>79</v>
       </c>
@@ -10370,7 +10365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="53" t="s">
         <v>80</v>
       </c>
@@ -10431,22 +10426,22 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="58.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -10481,7 +10476,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>29</v>
       </c>
@@ -10498,7 +10493,7 @@
       <c r="J2" s="96"/>
       <c r="K2" s="96"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>86</v>
       </c>
@@ -10515,7 +10510,7 @@
       <c r="J3" s="96"/>
       <c r="K3" s="96"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>61</v>
       </c>
@@ -10532,7 +10527,7 @@
       <c r="J4" s="96"/>
       <c r="K4" s="96"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>149</v>
       </c>
@@ -10549,7 +10544,7 @@
       <c r="J5" s="96"/>
       <c r="K5" s="96"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>197</v>
       </c>
@@ -10568,7 +10563,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>63</v>
       </c>
@@ -10587,7 +10582,7 @@
       <c r="J7" s="96"/>
       <c r="K7" s="96"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>64</v>
       </c>
@@ -10606,7 +10601,7 @@
       <c r="J8" s="96"/>
       <c r="K8" s="96"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>62</v>
       </c>
@@ -10625,7 +10620,7 @@
       <c r="J9" s="96"/>
       <c r="K9" s="96"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
         <v>190</v>
       </c>
@@ -10642,7 +10637,7 @@
       <c r="J10" s="96"/>
       <c r="K10" s="96"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="61" t="s">
         <v>207</v>
       </c>
@@ -10659,7 +10654,7 @@
       <c r="J11" s="96"/>
       <c r="K11" s="96"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>191</v>
       </c>
@@ -10676,7 +10671,7 @@
       <c r="J12" s="96"/>
       <c r="K12" s="96"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="61" t="s">
         <v>192</v>
       </c>
@@ -10693,7 +10688,7 @@
       <c r="J13" s="96"/>
       <c r="K13" s="96"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="98" t="s">
         <v>189</v>
       </c>
@@ -10712,7 +10707,7 @@
       <c r="J14" s="96"/>
       <c r="K14" s="96"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="98" t="s">
         <v>206</v>
       </c>
@@ -10731,7 +10726,7 @@
       <c r="J15" s="96"/>
       <c r="K15" s="96"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
         <v>57</v>
       </c>
@@ -10752,7 +10747,7 @@
       <c r="J16" s="96"/>
       <c r="K16" s="96"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>47</v>
       </c>
@@ -10769,7 +10764,7 @@
       <c r="J17" s="96"/>
       <c r="K17" s="96"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>175</v>
       </c>
@@ -10788,7 +10783,7 @@
       <c r="J18" s="96"/>
       <c r="K18" s="96"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
         <v>174</v>
       </c>
@@ -10807,7 +10802,7 @@
       <c r="J19" s="96"/>
       <c r="K19" s="96"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="53" t="s">
         <v>173</v>
       </c>
@@ -10826,7 +10821,7 @@
       <c r="J20" s="96"/>
       <c r="K20" s="96"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>196</v>
       </c>
@@ -10845,7 +10840,7 @@
       <c r="J21" s="96"/>
       <c r="K21" s="96"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
         <v>136</v>
       </c>
@@ -10866,7 +10861,7 @@
       <c r="J22" s="96"/>
       <c r="K22" s="96"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>34</v>
       </c>
@@ -10885,7 +10880,7 @@
       <c r="J23" s="96"/>
       <c r="K23" s="96"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>88</v>
       </c>
@@ -10902,7 +10897,7 @@
       <c r="J24" s="96"/>
       <c r="K24" s="96"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>87</v>
       </c>
@@ -10919,7 +10914,7 @@
       <c r="J25" s="96"/>
       <c r="K25" s="96"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>137</v>
       </c>
@@ -10936,7 +10931,7 @@
       <c r="J26" s="96"/>
       <c r="K26" s="96"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>59</v>
       </c>
@@ -10955,7 +10950,7 @@
       <c r="J27" s="96"/>
       <c r="K27" s="96"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>84</v>
       </c>
@@ -11177,22 +11172,22 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="16.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>217</v>
       </c>
@@ -11227,7 +11222,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -11256,7 +11251,7 @@
       <c r="J2" s="96"/>
       <c r="K2" s="96"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -11285,7 +11280,7 @@
       <c r="J3" s="96"/>
       <c r="K3" s="96"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -11314,7 +11309,7 @@
       <c r="J4" s="96"/>
       <c r="K4" s="96"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
@@ -11343,7 +11338,7 @@
       <c r="J5" s="96"/>
       <c r="K5" s="96"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
@@ -11372,7 +11367,7 @@
       <c r="J6" s="96"/>
       <c r="K6" s="96"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>53</v>
       </c>
@@ -11393,7 +11388,7 @@
       <c r="J7" s="96"/>
       <c r="K7" s="96"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>54</v>
       </c>
@@ -11414,7 +11409,7 @@
       <c r="J8" s="96"/>
       <c r="K8" s="96"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>55</v>
       </c>
@@ -11435,7 +11430,7 @@
       <c r="J9" s="96"/>
       <c r="K9" s="96"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
@@ -11456,7 +11451,7 @@
       <c r="J10" s="96"/>
       <c r="K10" s="96"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>49</v>
       </c>
@@ -11477,7 +11472,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>50</v>
       </c>
@@ -11496,7 +11491,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>51</v>
       </c>
@@ -11515,7 +11510,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>52</v>
       </c>
@@ -11551,15 +11546,15 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="48.08984375" style="35" customWidth="1"/>
     <col min="2" max="2" width="15" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="12.77734375" style="35"/>
+    <col min="3" max="3" width="14.6328125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>218</v>
       </c>
@@ -11585,7 +11580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>219</v>
       </c>
@@ -11611,7 +11606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="143"/>
       <c r="C3" s="35" t="s">
         <v>177</v>
@@ -11633,7 +11628,7 @@
       </c>
       <c r="J3" s="106"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B4" s="143"/>
       <c r="C4" s="35" t="s">
         <v>176</v>
@@ -11655,7 +11650,7 @@
       </c>
       <c r="J4" s="106"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="143" t="s">
         <v>1</v>
       </c>
@@ -11679,7 +11674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B6" s="143"/>
       <c r="C6" s="35" t="s">
         <v>177</v>
@@ -11700,7 +11695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B7" s="143"/>
       <c r="C7" s="35" t="s">
         <v>176</v>
@@ -11721,7 +11716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B8" s="143" t="s">
         <v>2</v>
       </c>
@@ -11744,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B9" s="143"/>
       <c r="C9" s="35" t="s">
         <v>177</v>
@@ -11765,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B10" s="143"/>
       <c r="C10" s="35" t="s">
         <v>176</v>
@@ -11786,7 +11781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="143" t="s">
         <v>3</v>
       </c>
@@ -11809,7 +11804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B12" s="143"/>
       <c r="C12" s="35" t="s">
         <v>177</v>
@@ -11830,7 +11825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B13" s="143"/>
       <c r="C13" s="35" t="s">
         <v>176</v>
@@ -11851,7 +11846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B14" s="143" t="s">
         <v>4</v>
       </c>
@@ -11874,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B15" s="143"/>
       <c r="C15" s="35" t="s">
         <v>177</v>
@@ -11895,7 +11890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B16" s="143"/>
       <c r="C16" s="35" t="s">
         <v>176</v>
@@ -11916,7 +11911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B17" s="107" t="s">
         <v>172</v>
       </c>
@@ -11939,14 +11934,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="D18" s="108"/>
       <c r="E18" s="108"/>
       <c r="F18" s="108"/>
       <c r="G18" s="108"/>
       <c r="H18" s="108"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>220</v>
       </c>
@@ -11972,7 +11967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B20" s="143"/>
       <c r="C20" s="35" t="s">
         <v>177</v>
@@ -11993,7 +11988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B21" s="143"/>
       <c r="C21" s="35" t="s">
         <v>176</v>
@@ -12014,7 +12009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B22" s="143" t="s">
         <v>1</v>
       </c>
@@ -12037,7 +12032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B23" s="143"/>
       <c r="C23" s="35" t="s">
         <v>177</v>
@@ -12058,7 +12053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B24" s="143"/>
       <c r="C24" s="35" t="s">
         <v>176</v>
@@ -12079,7 +12074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B25" s="143" t="s">
         <v>2</v>
       </c>
@@ -12102,7 +12097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B26" s="143"/>
       <c r="C26" s="35" t="s">
         <v>177</v>
@@ -12123,7 +12118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B27" s="143"/>
       <c r="C27" s="35" t="s">
         <v>176</v>
@@ -12144,7 +12139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B28" s="143" t="s">
         <v>3</v>
       </c>
@@ -12167,7 +12162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B29" s="143"/>
       <c r="C29" s="35" t="s">
         <v>177</v>
@@ -12188,7 +12183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B30" s="143"/>
       <c r="C30" s="35" t="s">
         <v>176</v>
@@ -12209,7 +12204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B31" s="143" t="s">
         <v>4</v>
       </c>
@@ -12232,7 +12227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B32" s="143"/>
       <c r="C32" s="35" t="s">
         <v>177</v>
@@ -12253,7 +12248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B33" s="143"/>
       <c r="C33" s="35" t="s">
         <v>176</v>
@@ -12274,7 +12269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B34" s="107" t="s">
         <v>172</v>
       </c>
@@ -12304,7 +12299,7 @@
       <c r="G35" s="108"/>
       <c r="H35" s="108"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="109" t="s">
         <v>221</v>
       </c>
@@ -12632,7 +12627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B51" s="110" t="s">
         <v>172</v>
       </c>
@@ -12658,12 +12653,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12673,6 +12662,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12690,22 +12685,22 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="34.08984375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="35" customWidth="1"/>
     <col min="5" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="16.109375" style="35"/>
+    <col min="7" max="16384" width="16.08984375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="112" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="112" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="111" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="113"/>
       <c r="C2" s="114" t="s">
         <v>26</v>
@@ -12720,7 +12715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>223</v>
       </c>
@@ -12804,7 +12799,7 @@
       <c r="E8" s="106"/>
       <c r="F8" s="106"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
         <v>224</v>
       </c>
@@ -12829,7 +12824,7 @@
       <c r="F10" s="106"/>
       <c r="G10" s="123"/>
     </row>
-    <row r="11" spans="1:7" s="112" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="112" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="111" t="s">
         <v>225</v>
       </c>
@@ -12839,7 +12834,7 @@
       <c r="F11" s="125"/>
       <c r="G11" s="126"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
         <v>226</v>
       </c>
@@ -12903,7 +12898,7 @@
       </c>
       <c r="G15" s="123"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="40"/>
       <c r="B16" s="127"/>
       <c r="C16" s="128"/>
@@ -12912,7 +12907,7 @@
       <c r="F16" s="106"/>
       <c r="G16" s="123"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
         <v>230</v>
       </c>
@@ -13066,7 +13061,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="127"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="40"/>
     </row>
   </sheetData>
@@ -13087,23 +13082,23 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.21875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="35" customWidth="1"/>
-    <col min="4" max="8" width="14.77734375" style="35" customWidth="1"/>
-    <col min="9" max="12" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="27.1796875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" style="35" customWidth="1"/>
+    <col min="4" max="8" width="14.81640625" style="35" customWidth="1"/>
+    <col min="9" max="12" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="16.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="111" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="132" t="s">
         <v>211</v>
       </c>
@@ -13137,7 +13132,7 @@
       <c r="O2" s="134"/>
       <c r="P2" s="134"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="35" t="s">
         <v>71</v>
@@ -13570,7 +13565,7 @@
       <c r="O17" s="132"/>
       <c r="P17" s="132"/>
     </row>
-    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="43" t="s">
         <v>237</v>
       </c>
@@ -13828,12 +13823,12 @@
       <c r="O26" s="132"/>
       <c r="P26" s="132"/>
     </row>
-    <row r="28" spans="1:16" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="111" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="135" t="s">
         <v>239</v>
       </c>
@@ -13867,7 +13862,7 @@
       <c r="O29" s="134"/>
       <c r="P29" s="134"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="35" t="s">
         <v>71</v>
@@ -14562,12 +14557,12 @@
       <c r="C54" s="43"/>
       <c r="D54" s="43"/>
     </row>
-    <row r="55" spans="1:16" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="111" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A56" s="135" t="s">
         <v>70</v>
       </c>
@@ -14595,7 +14590,7 @@
       <c r="O56" s="134"/>
       <c r="P56" s="134"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="35" t="s">
         <v>38</v>
@@ -14741,12 +14736,12 @@
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
     </row>
-    <row r="64" spans="1:16" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="111" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A65" s="135" t="s">
         <v>24</v>
       </c>
@@ -14780,7 +14775,7 @@
       <c r="O65" s="134"/>
       <c r="P65" s="134"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="139"/>
       <c r="B66" s="35" t="s">
         <v>73</v>
@@ -15816,12 +15811,12 @@
       <c r="O101" s="132"/>
       <c r="P101" s="132"/>
     </row>
-    <row r="103" spans="1:16" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A103" s="111" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A104" s="135" t="s">
         <v>71</v>
       </c>
@@ -15855,7 +15850,7 @@
       <c r="O104" s="134"/>
       <c r="P104" s="134"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="36"/>
       <c r="C105" s="43" t="s">
@@ -15969,7 +15964,7 @@
       <c r="O108" s="132"/>
       <c r="P108" s="132"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
     </row>
   </sheetData>
@@ -15990,14 +15985,14 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="12" customWidth="1"/>
-    <col min="2" max="9" width="16.77734375" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="14.44140625" style="12"/>
+    <col min="1" max="1" width="8.453125" style="12" customWidth="1"/>
+    <col min="2" max="9" width="16.81640625" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="14.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -16946,24 +16941,24 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="44.44140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="35" customWidth="1"/>
     <col min="6" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="7" max="7" width="13.6328125" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="111" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="139" t="s">
         <v>25</v>
       </c>
@@ -17004,7 +16999,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="131" t="s">
         <v>251</v>
@@ -17025,7 +17020,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="116" t="s">
         <v>252</v>
       </c>
@@ -17098,12 +17093,12 @@
       <c r="F9" s="131"/>
       <c r="G9" s="131"/>
     </row>
-    <row r="10" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="111" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="116"/>
       <c r="B11" s="127" t="s">
         <v>196</v>
@@ -17124,16 +17119,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="116"/>
       <c r="B12" s="127"/>
     </row>
-    <row r="13" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="111" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="139" t="s">
         <v>239</v>
       </c>
@@ -17156,7 +17151,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="131" t="s">
         <v>256</v>
@@ -17177,7 +17172,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="139" t="s">
         <v>70</v>
       </c>
@@ -17201,12 +17196,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="111" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="116" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="116" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="57" t="s">
         <v>49</v>
       </c>
@@ -17256,16 +17251,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.21875" style="35" customWidth="1"/>
-    <col min="2" max="6" width="16.109375" style="35"/>
-    <col min="7" max="7" width="17.21875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="16.109375" style="35"/>
+    <col min="1" max="1" width="52.1796875" style="35" customWidth="1"/>
+    <col min="2" max="6" width="16.08984375" style="35"/>
+    <col min="7" max="7" width="17.1796875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="16.08984375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="133" t="s">
         <v>69</v>
       </c>
@@ -17535,15 +17530,15 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="58.90625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="15" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="12.77734375" style="35"/>
+    <col min="16" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="115" t="s">
@@ -17586,7 +17581,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>261</v>
       </c>
@@ -18031,7 +18026,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="61" t="s">
         <v>137</v>
       </c>
@@ -18119,7 +18114,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>262</v>
       </c>
@@ -18331,15 +18326,15 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" style="35" customWidth="1"/>
-    <col min="3" max="7" width="15.5546875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="21.36328125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="35" customWidth="1"/>
+    <col min="3" max="7" width="15.54296875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40"/>
       <c r="B1" s="133"/>
       <c r="C1" s="40" t="s">
@@ -18358,12 +18353,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="61" t="s">
         <v>67</v>
       </c>
@@ -18383,7 +18378,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>264</v>
       </c>
@@ -18394,7 +18389,7 @@
       <c r="F4" s="141"/>
       <c r="G4" s="141"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="98" t="s">
         <v>185</v>
       </c>
@@ -18432,20 +18427,20 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="53" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="53" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" style="53" customWidth="1"/>
     <col min="4" max="4" width="15" style="35" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="35" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="35"/>
-    <col min="8" max="8" width="17.5546875" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="12.77734375" style="35"/>
+    <col min="5" max="5" width="13.6328125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="35"/>
+    <col min="8" max="8" width="17.54296875" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -18471,7 +18466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>28</v>
       </c>
@@ -18497,7 +18492,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C3" s="53" t="s">
         <v>268</v>
       </c>
@@ -18517,7 +18512,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C4" s="53" t="s">
         <v>269</v>
       </c>
@@ -18537,7 +18532,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>58</v>
       </c>
@@ -18563,7 +18558,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C6" s="53" t="s">
         <v>269</v>
       </c>
@@ -18583,7 +18578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B7" s="53" t="s">
         <v>65</v>
       </c>
@@ -18606,7 +18601,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C8" s="53" t="s">
         <v>269</v>
       </c>
@@ -18626,7 +18621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>136</v>
       </c>
@@ -18652,7 +18647,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C10" s="53" t="s">
         <v>269</v>
       </c>
@@ -18672,7 +18667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="53" t="s">
         <v>65</v>
       </c>
@@ -18695,7 +18690,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C12" s="53" t="s">
         <v>269</v>
       </c>
@@ -18715,7 +18710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>61</v>
       </c>
@@ -18741,7 +18736,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C14" s="53" t="s">
         <v>269</v>
       </c>
@@ -18762,7 +18757,7 @@
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B15" s="53" t="s">
         <v>65</v>
       </c>
@@ -18786,7 +18781,7 @@
       </c>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C16" s="53" t="s">
         <v>269</v>
       </c>
@@ -18807,7 +18802,7 @@
       </c>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>62</v>
       </c>
@@ -18834,7 +18829,7 @@
       </c>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C18" s="53" t="s">
         <v>268</v>
       </c>
@@ -18855,7 +18850,7 @@
       </c>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
         <v>63</v>
       </c>
@@ -18881,7 +18876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C20" s="53" t="s">
         <v>268</v>
       </c>
@@ -18901,7 +18896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>64</v>
       </c>
@@ -18927,7 +18922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C22" s="53" t="s">
         <v>268</v>
       </c>
@@ -18947,7 +18942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>79</v>
       </c>
@@ -18973,7 +18968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C24" s="53" t="s">
         <v>268</v>
       </c>
@@ -18993,7 +18988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C25" s="53" t="s">
         <v>269</v>
       </c>
@@ -19013,7 +19008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>80</v>
       </c>
@@ -19039,7 +19034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C27" s="53" t="s">
         <v>268</v>
       </c>
@@ -19059,7 +19054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C28" s="53" t="s">
         <v>269</v>
       </c>
@@ -19079,7 +19074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="53" t="s">
         <v>81</v>
       </c>
@@ -19105,7 +19100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C30" s="53" t="s">
         <v>268</v>
       </c>
@@ -19125,7 +19120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C31" s="53" t="s">
         <v>269</v>
       </c>
@@ -19145,7 +19140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
         <v>82</v>
       </c>
@@ -19171,7 +19166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C33" s="53" t="s">
         <v>268</v>
       </c>
@@ -19191,7 +19186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C34" s="53" t="s">
         <v>269</v>
       </c>
@@ -19211,7 +19206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>83</v>
       </c>
@@ -19237,7 +19232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C36" s="53" t="s">
         <v>268</v>
       </c>
@@ -19257,7 +19252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C37" s="53" t="s">
         <v>269</v>
       </c>
@@ -19277,7 +19272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
         <v>60</v>
       </c>
@@ -19303,7 +19298,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C39" s="53" t="s">
         <v>268</v>
       </c>
@@ -19323,7 +19318,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C40" s="53" t="s">
         <v>269</v>
       </c>
@@ -19343,7 +19338,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B41" s="53" t="s">
         <v>16</v>
       </c>
@@ -19366,7 +19361,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C42" s="53" t="s">
         <v>268</v>
       </c>
@@ -19386,7 +19381,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C43" s="53" t="s">
         <v>269</v>
       </c>
@@ -19406,7 +19401,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A44" s="53" t="s">
         <v>84</v>
       </c>
@@ -19432,7 +19427,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C45" s="53" t="s">
         <v>268</v>
       </c>
@@ -19452,7 +19447,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
         <v>85</v>
       </c>
@@ -19478,7 +19473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C47" s="53" t="s">
         <v>268</v>
       </c>
@@ -19498,7 +19493,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
         <v>196</v>
       </c>
@@ -19524,7 +19519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C49" s="53" t="s">
         <v>268</v>
       </c>
@@ -19562,16 +19557,16 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="35" customWidth="1"/>
-    <col min="4" max="7" width="17.21875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="2" max="2" width="27.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" style="35" customWidth="1"/>
+    <col min="4" max="7" width="17.1796875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="133" t="s">
         <v>69</v>
       </c>
@@ -19593,7 +19588,7 @@
       </c>
       <c r="H1" s="104"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>86</v>
       </c>
@@ -19617,7 +19612,7 @@
       </c>
       <c r="H2" s="98"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C3" s="35" t="s">
         <v>268</v>
       </c>
@@ -19635,7 +19630,7 @@
       </c>
       <c r="H3" s="142"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>87</v>
       </c>
@@ -19659,7 +19654,7 @@
       </c>
       <c r="H4" s="142"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="C5" s="35" t="s">
         <v>268</v>
@@ -19678,7 +19673,7 @@
       </c>
       <c r="H5" s="98"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>88</v>
       </c>
@@ -19702,7 +19697,7 @@
       </c>
       <c r="H6" s="98"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="C7" s="35" t="s">
         <v>268</v>
@@ -19735,7 +19730,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
@@ -19773,16 +19768,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="35" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" style="35"/>
-    <col min="5" max="5" width="17.44140625" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="35"/>
+    <col min="1" max="1" width="33.6328125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" style="35"/>
+    <col min="5" max="5" width="17.453125" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>163</v>
       </c>
@@ -19799,7 +19794,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
@@ -19817,7 +19812,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>157</v>
       </c>
@@ -19835,7 +19830,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>156</v>
       </c>
@@ -19853,7 +19848,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>155</v>
       </c>
@@ -19871,7 +19866,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -19889,7 +19884,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>153</v>
       </c>
@@ -19907,7 +19902,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>152</v>
       </c>
@@ -19925,7 +19920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>151</v>
       </c>
@@ -19943,7 +19938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>150</v>
       </c>
@@ -19982,14 +19977,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -20000,7 +19995,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -20083,7 +20078,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -20217,7 +20212,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -20315,13 +20310,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -20379,23 +20374,23 @@
         <v>118</v>
       </c>
       <c r="C3" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
         <v/>
       </c>
       <c r="D3" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
         <v/>
       </c>
       <c r="E3" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
         <v/>
       </c>
       <c r="F3" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
         <v/>
       </c>
       <c r="G3" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
         <v/>
       </c>
     </row>
@@ -20470,23 +20465,23 @@
         <v>121</v>
       </c>
       <c r="C9" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
         <v/>
       </c>
       <c r="D9" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
         <v/>
       </c>
       <c r="E9" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
         <v/>
       </c>
       <c r="F9" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
         <v/>
       </c>
       <c r="G9" s="77" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
         <v/>
       </c>
     </row>
@@ -20676,13 +20671,13 @@
       <selection activeCell="C2" sqref="C2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
-    <col min="2" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -20775,17 +20770,19 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -20793,41 +20790,71 @@
         <v>145</v>
       </c>
       <c r="C1">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="D1">
-        <v>2011</v>
+        <f>C1+1</f>
+        <v>2018</v>
       </c>
       <c r="E1">
-        <v>2012</v>
+        <f t="shared" ref="E1:N1" si="0">D1+1</f>
+        <v>2019</v>
       </c>
       <c r="F1">
-        <v>2013</v>
+        <f t="shared" si="0"/>
+        <v>2020</v>
       </c>
       <c r="G1">
-        <v>2014</v>
+        <f t="shared" si="0"/>
+        <v>2021</v>
       </c>
       <c r="H1">
-        <v>2015</v>
+        <f t="shared" si="0"/>
+        <v>2022</v>
       </c>
       <c r="I1">
-        <v>2016</v>
+        <f t="shared" si="0"/>
+        <v>2023</v>
       </c>
       <c r="J1">
-        <v>2017</v>
+        <f t="shared" si="0"/>
+        <v>2024</v>
       </c>
       <c r="K1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="O1">
+        <f>N1+1</f>
+        <v>2029</v>
+      </c>
+      <c r="P1">
+        <f>O1+1</f>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="28">
+        <v>0.2</v>
+      </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
@@ -20836,18 +20863,27 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="28">
+        <v>0.25</v>
+      </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -20856,18 +20892,27 @@
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="28">
+        <v>0.15</v>
+      </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
@@ -20876,12 +20921,21 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="28">
+        <v>0.25</v>
+      </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
@@ -20890,12 +20944,21 @@
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="28">
+        <v>0.2</v>
+      </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
@@ -20904,15 +20967,24 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="28">
+        <v>0.45</v>
+      </c>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -20921,12 +20993,21 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="28">
+        <v>0.35</v>
+      </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
@@ -20935,15 +21016,24 @@
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="28">
+        <v>0.1</v>
+      </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -20952,12 +21042,21 @@
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="28">
+        <v>0.05</v>
+      </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
@@ -20966,6 +21065,13 @@
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28">
+        <v>0.02</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20984,15 +21090,15 @@
       <selection activeCell="E21" activeCellId="5" sqref="C2:D6 E7 C9:D13 E14 C16:D20 E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="35" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="35"/>
+    <col min="2" max="2" width="19.08984375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>180</v>
       </c>
@@ -21009,7 +21115,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>175</v>
       </c>
@@ -21023,7 +21129,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="46" t="s">
         <v>1</v>
@@ -21035,7 +21141,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="46" t="s">
         <v>2</v>
@@ -21047,7 +21153,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="46" t="s">
         <v>3</v>
@@ -21059,7 +21165,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="46" t="s">
         <v>4</v>
@@ -21071,7 +21177,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="46" t="s">
         <v>172</v>
@@ -21080,7 +21186,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="81"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>174</v>
       </c>
@@ -21091,7 +21197,7 @@
       <c r="D9" s="81"/>
       <c r="E9" s="59"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="46" t="s">
         <v>1</v>
@@ -21100,7 +21206,7 @@
       <c r="D10" s="81"/>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="46" t="s">
         <v>2</v>
@@ -21109,7 +21215,7 @@
       <c r="D11" s="81"/>
       <c r="E11" s="58"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="46" t="s">
         <v>3</v>
@@ -21118,7 +21224,7 @@
       <c r="D12" s="81"/>
       <c r="E12" s="58"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="46" t="s">
         <v>4</v>
@@ -21127,7 +21233,7 @@
       <c r="D13" s="81"/>
       <c r="E13" s="58"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="46" t="s">
         <v>172</v>
@@ -21136,7 +21242,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="81"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
         <v>173</v>
       </c>
@@ -21150,7 +21256,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="46" t="s">
         <v>1</v>
@@ -21162,7 +21268,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="46" t="s">
         <v>2</v>
@@ -21174,7 +21280,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="46" t="s">
         <v>3</v>
@@ -21186,7 +21292,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="46" t="s">
         <v>4</v>
@@ -21198,7 +21304,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="46" t="s">
         <v>172</v>
@@ -21225,15 +21331,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="62" t="s">
         <v>164</v>
       </c>
@@ -21247,7 +21353,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
         <v>69</v>
       </c>
@@ -21259,7 +21365,7 @@
       </c>
       <c r="D2" s="81"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
         <v>187</v>
       </c>
@@ -21288,17 +21394,17 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="53" customWidth="1"/>
     <col min="2" max="2" width="20" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.44140625" style="35"/>
+    <col min="3" max="3" width="20.453125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="32.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Separated management of MAM as a program
</commit_message>
<xml_diff>
--- a/inputs/template_input.xlsx
+++ b/inputs/template_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07AF228-F632-4835-8A14-F90E7236A652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -45,6 +46,8 @@
     <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$38</definedName>
     <definedName name="abortion">'Baseline year population inputs'!$C$41</definedName>
     <definedName name="comm_deliv">'Treatment of SAM'!$D$3</definedName>
+    <definedName name="comm_deliv_mam">'Treatment of SAM'!$D$3</definedName>
+    <definedName name="comm_deliv_sam">'Treatment of SAM'!$D$2</definedName>
     <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$52</definedName>
     <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$54</definedName>
     <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$51</definedName>
@@ -90,17 +93,27 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -148,11 +161,37 @@
           <t xml:space="preserve">
 The cost per child per year can be estimated as 
 = (cost per treatment episode) * (SAM prevalence) * 2.6
-Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
+See user guide for further information</t>
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{E41DC1AA-D6CD-4883-9D64-BC2E05F0B407}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The cost per child per year can be estimated as 
+= (cost per treatment episode) * (MAM prevalence) * 2.6
+See user guide for further information</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -183,12 +222,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -241,12 +280,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -275,12 +314,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -304,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -334,12 +373,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -377,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="270">
   <si>
     <t>year</t>
   </si>
@@ -1192,7 +1231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2934,7 +2973,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3264,10 +3303,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1450">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="1449"/>
+    <cellStyle name="Comma 2" xfId="1449" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4713,8 +4753,8 @@
     <cellStyle name="Hyperlink" xfId="1445" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1447" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000A7050000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000A8050000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -6154,7 +6194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -6546,14 +6586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6721,7 +6761,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6819,7 +6859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -6933,14 +6973,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7337,19 +7377,19 @@
         <v>0</v>
       </c>
       <c r="D9" s="93">
-        <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
+        <f>IF(ISBLANK(comm_deliv_sam), frac_children_health_facility,1)</f>
         <v>0</v>
       </c>
       <c r="E9" s="93">
-        <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
+        <f>IF(ISBLANK(comm_deliv_sam), frac_children_health_facility,1)</f>
         <v>0</v>
       </c>
       <c r="F9" s="93">
-        <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
+        <f>IF(ISBLANK(comm_deliv_sam), frac_children_health_facility,1)</f>
         <v>0</v>
       </c>
       <c r="G9" s="93">
-        <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
+        <f>IF(ISBLANK(comm_deliv_sam), frac_children_health_facility,1)</f>
         <v>0</v>
       </c>
       <c r="H9" s="94">
@@ -7377,228 +7417,231 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="93">
+        <v>0</v>
+      </c>
+      <c r="D10" s="93">
+        <f>IF(ISBLANK(comm_deliv_mam), frac_children_health_facility,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="93">
+        <f>IF(ISBLANK(comm_deliv_mam), frac_children_health_facility,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="93">
+        <f>IF(ISBLANK(comm_deliv_mam), frac_children_health_facility,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="93">
+        <f>IF(ISBLANK(comm_deliv_mam), frac_children_health_facility,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="94">
+        <v>0</v>
+      </c>
+      <c r="I10" s="94">
+        <v>0</v>
+      </c>
+      <c r="J10" s="94">
+        <v>0</v>
+      </c>
+      <c r="K10" s="94">
+        <v>0</v>
+      </c>
+      <c r="L10" s="94">
+        <v>0</v>
+      </c>
+      <c r="M10" s="94">
+        <v>0</v>
+      </c>
+      <c r="N10" s="94">
+        <v>0</v>
+      </c>
+      <c r="O10" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="93">
-        <v>0</v>
-      </c>
-      <c r="D10" s="93">
-        <v>0</v>
-      </c>
-      <c r="E10" s="93">
-        <v>1</v>
-      </c>
-      <c r="F10" s="93">
-        <v>1</v>
-      </c>
-      <c r="G10" s="93">
-        <v>1</v>
-      </c>
-      <c r="H10" s="94">
-        <v>0</v>
-      </c>
-      <c r="I10" s="94">
-        <v>0</v>
-      </c>
-      <c r="J10" s="94">
-        <v>0</v>
-      </c>
-      <c r="K10" s="94">
-        <v>0</v>
-      </c>
-      <c r="L10" s="94">
-        <v>0</v>
-      </c>
-      <c r="M10" s="94">
-        <v>0</v>
-      </c>
-      <c r="N10" s="94">
-        <v>0</v>
-      </c>
-      <c r="O10" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="C11" s="93">
+        <v>0</v>
+      </c>
+      <c r="D11" s="93">
+        <v>0</v>
+      </c>
+      <c r="E11" s="93">
+        <v>1</v>
+      </c>
+      <c r="F11" s="93">
+        <v>1</v>
+      </c>
+      <c r="G11" s="93">
+        <v>1</v>
+      </c>
+      <c r="H11" s="94">
+        <v>0</v>
+      </c>
+      <c r="I11" s="94">
+        <v>0</v>
+      </c>
+      <c r="J11" s="94">
+        <v>0</v>
+      </c>
+      <c r="K11" s="94">
+        <v>0</v>
+      </c>
+      <c r="L11" s="94">
+        <v>0</v>
+      </c>
+      <c r="M11" s="94">
+        <v>0</v>
+      </c>
+      <c r="N11" s="94">
+        <v>0</v>
+      </c>
+      <c r="O11" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C12" s="93">
         <f>diarrhoea_1mo/26</f>
         <v>0</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D12" s="93">
         <f>diarrhoea_1_5mo/26</f>
         <v>0</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E12" s="93">
         <f>diarrhoea_6_11mo/26</f>
         <v>0</v>
       </c>
-      <c r="F11" s="93">
+      <c r="F12" s="93">
         <f>diarrhoea_12_23mo/26</f>
         <v>0</v>
       </c>
-      <c r="G11" s="93">
+      <c r="G12" s="93">
         <f>diarrhoea_24_59mo/26</f>
         <v>0</v>
       </c>
-      <c r="H11" s="94">
-        <v>0</v>
-      </c>
-      <c r="I11" s="94">
-        <v>0</v>
-      </c>
-      <c r="J11" s="94">
-        <v>0</v>
-      </c>
-      <c r="K11" s="94">
-        <v>0</v>
-      </c>
-      <c r="L11" s="94">
-        <v>0</v>
-      </c>
-      <c r="M11" s="94">
-        <v>0</v>
-      </c>
-      <c r="N11" s="94">
-        <v>0</v>
-      </c>
-      <c r="O11" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="H12" s="94">
+        <v>0</v>
+      </c>
+      <c r="I12" s="94">
+        <v>0</v>
+      </c>
+      <c r="J12" s="94">
+        <v>0</v>
+      </c>
+      <c r="K12" s="94">
+        <v>0</v>
+      </c>
+      <c r="L12" s="94">
+        <v>0</v>
+      </c>
+      <c r="M12" s="94">
+        <v>0</v>
+      </c>
+      <c r="N12" s="94">
+        <v>0</v>
+      </c>
+      <c r="O12" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="93">
-        <v>0</v>
-      </c>
-      <c r="D12" s="93">
-        <v>0</v>
-      </c>
-      <c r="E12" s="93">
-        <v>1</v>
-      </c>
-      <c r="F12" s="93">
-        <v>1</v>
-      </c>
-      <c r="G12" s="93">
-        <v>1</v>
-      </c>
-      <c r="H12" s="94">
-        <v>0</v>
-      </c>
-      <c r="I12" s="94">
-        <v>0</v>
-      </c>
-      <c r="J12" s="94">
-        <v>0</v>
-      </c>
-      <c r="K12" s="94">
-        <v>0</v>
-      </c>
-      <c r="L12" s="94">
-        <v>0</v>
-      </c>
-      <c r="M12" s="94">
-        <v>0</v>
-      </c>
-      <c r="N12" s="94">
-        <v>0</v>
-      </c>
-      <c r="O12" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="C13" s="93">
+        <v>0</v>
+      </c>
+      <c r="D13" s="93">
+        <v>0</v>
+      </c>
+      <c r="E13" s="93">
+        <v>1</v>
+      </c>
+      <c r="F13" s="93">
+        <v>1</v>
+      </c>
+      <c r="G13" s="93">
+        <v>1</v>
+      </c>
+      <c r="H13" s="94">
+        <v>0</v>
+      </c>
+      <c r="I13" s="94">
+        <v>0</v>
+      </c>
+      <c r="J13" s="94">
+        <v>0</v>
+      </c>
+      <c r="K13" s="94">
+        <v>0</v>
+      </c>
+      <c r="L13" s="94">
+        <v>0</v>
+      </c>
+      <c r="M13" s="94">
+        <v>0</v>
+      </c>
+      <c r="N13" s="94">
+        <v>0</v>
+      </c>
+      <c r="O13" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="33"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="94">
-        <v>0</v>
-      </c>
-      <c r="D14" s="94">
-        <v>0</v>
-      </c>
-      <c r="E14" s="94">
-        <v>0</v>
-      </c>
-      <c r="F14" s="94">
-        <v>0</v>
-      </c>
-      <c r="G14" s="94">
-        <v>0</v>
-      </c>
-      <c r="H14" s="93">
+      <c r="C15" s="94">
+        <v>0</v>
+      </c>
+      <c r="D15" s="94">
+        <v>0</v>
+      </c>
+      <c r="E15" s="94">
+        <v>0</v>
+      </c>
+      <c r="F15" s="94">
+        <v>0</v>
+      </c>
+      <c r="G15" s="94">
+        <v>0</v>
+      </c>
+      <c r="H15" s="93">
         <f>food_insecure</f>
         <v>0</v>
       </c>
-      <c r="I14" s="93">
+      <c r="I15" s="93">
         <f>food_insecure</f>
         <v>0</v>
       </c>
-      <c r="J14" s="93">
+      <c r="J15" s="93">
         <f>food_insecure</f>
         <v>0</v>
       </c>
-      <c r="K14" s="93">
+      <c r="K15" s="93">
         <f>food_insecure</f>
         <v>0</v>
-      </c>
-      <c r="L14" s="94">
-        <v>0</v>
-      </c>
-      <c r="M14" s="94">
-        <v>0</v>
-      </c>
-      <c r="N14" s="94">
-        <v>0</v>
-      </c>
-      <c r="O14" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="94">
-        <v>0</v>
-      </c>
-      <c r="D15" s="94">
-        <v>0</v>
-      </c>
-      <c r="E15" s="94">
-        <v>0</v>
-      </c>
-      <c r="F15" s="94">
-        <v>0</v>
-      </c>
-      <c r="G15" s="94">
-        <v>0</v>
-      </c>
-      <c r="H15" s="93">
-        <v>1</v>
-      </c>
-      <c r="I15" s="93">
-        <v>1</v>
-      </c>
-      <c r="J15" s="93">
-        <v>1</v>
-      </c>
-      <c r="K15" s="93">
-        <v>1</v>
       </c>
       <c r="L15" s="94">
         <v>0</v>
@@ -7616,7 +7659,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
       <c r="C16" s="94">
         <v>0</v>
@@ -7634,19 +7677,15 @@
         <v>0</v>
       </c>
       <c r="H16" s="93">
-        <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
       <c r="I16" s="93">
-        <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
       <c r="J16" s="93">
-        <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
       <c r="K16" s="93">
-        <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
       <c r="L16" s="94">
@@ -7665,130 +7704,135 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="94">
+        <v>0</v>
+      </c>
+      <c r="D17" s="94">
+        <v>0</v>
+      </c>
+      <c r="E17" s="94">
+        <v>0</v>
+      </c>
+      <c r="F17" s="94">
+        <v>0</v>
+      </c>
+      <c r="G17" s="94">
+        <v>0</v>
+      </c>
+      <c r="H17" s="93">
+        <f xml:space="preserve"> 1</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="93">
+        <f xml:space="preserve"> 1</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="93">
+        <f xml:space="preserve"> 1</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="93">
+        <f xml:space="preserve"> 1</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="94">
+        <v>0</v>
+      </c>
+      <c r="M17" s="94">
+        <v>0</v>
+      </c>
+      <c r="N17" s="94">
+        <v>0</v>
+      </c>
+      <c r="O17" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="94">
-        <v>0</v>
-      </c>
-      <c r="D17" s="94">
-        <v>0</v>
-      </c>
-      <c r="E17" s="94">
-        <v>0</v>
-      </c>
-      <c r="F17" s="94">
-        <v>0</v>
-      </c>
-      <c r="G17" s="94">
-        <v>0</v>
-      </c>
-      <c r="H17" s="93">
+      <c r="C18" s="94">
+        <v>0</v>
+      </c>
+      <c r="D18" s="94">
+        <v>0</v>
+      </c>
+      <c r="E18" s="94">
+        <v>0</v>
+      </c>
+      <c r="F18" s="94">
+        <v>0</v>
+      </c>
+      <c r="G18" s="94">
+        <v>0</v>
+      </c>
+      <c r="H18" s="93">
         <f>frac_PW_health_facility</f>
         <v>0</v>
       </c>
-      <c r="I17" s="93">
+      <c r="I18" s="93">
         <f>frac_PW_health_facility</f>
         <v>0</v>
       </c>
-      <c r="J17" s="93">
+      <c r="J18" s="93">
         <f>frac_PW_health_facility</f>
         <v>0</v>
       </c>
-      <c r="K17" s="93">
+      <c r="K18" s="93">
         <f>frac_PW_health_facility</f>
         <v>0</v>
       </c>
-      <c r="L17" s="94">
-        <v>0</v>
-      </c>
-      <c r="M17" s="94">
-        <v>0</v>
-      </c>
-      <c r="N17" s="94">
-        <v>0</v>
-      </c>
-      <c r="O17" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
+      <c r="L18" s="94">
+        <v>0</v>
+      </c>
+      <c r="M18" s="94">
+        <v>0</v>
+      </c>
+      <c r="N18" s="94">
+        <v>0</v>
+      </c>
+      <c r="O18" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="94">
-        <v>0</v>
-      </c>
-      <c r="D18" s="94">
-        <v>0</v>
-      </c>
-      <c r="E18" s="94">
-        <v>0</v>
-      </c>
-      <c r="F18" s="94">
-        <v>0</v>
-      </c>
-      <c r="G18" s="94">
-        <v>0</v>
-      </c>
-      <c r="H18" s="93">
+      <c r="C19" s="94">
+        <v>0</v>
+      </c>
+      <c r="D19" s="94">
+        <v>0</v>
+      </c>
+      <c r="E19" s="94">
+        <v>0</v>
+      </c>
+      <c r="F19" s="94">
+        <v>0</v>
+      </c>
+      <c r="G19" s="94">
+        <v>0</v>
+      </c>
+      <c r="H19" s="93">
         <f>frac_malaria_risk</f>
         <v>0</v>
       </c>
-      <c r="I18" s="93">
+      <c r="I19" s="93">
         <f>frac_malaria_risk</f>
         <v>0</v>
       </c>
-      <c r="J18" s="93">
+      <c r="J19" s="93">
         <f>frac_malaria_risk</f>
         <v>0</v>
       </c>
-      <c r="K18" s="93">
+      <c r="K19" s="93">
         <f>frac_malaria_risk</f>
         <v>0</v>
-      </c>
-      <c r="L18" s="94">
-        <v>0</v>
-      </c>
-      <c r="M18" s="94">
-        <v>0</v>
-      </c>
-      <c r="N18" s="94">
-        <v>0</v>
-      </c>
-      <c r="O18" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="94">
-        <v>0</v>
-      </c>
-      <c r="D19" s="94">
-        <v>0</v>
-      </c>
-      <c r="E19" s="94">
-        <v>0</v>
-      </c>
-      <c r="F19" s="94">
-        <v>0</v>
-      </c>
-      <c r="G19" s="94">
-        <v>0</v>
-      </c>
-      <c r="H19" s="93">
-        <v>1</v>
-      </c>
-      <c r="I19" s="93">
-        <v>1</v>
-      </c>
-      <c r="J19" s="93">
-        <v>1</v>
-      </c>
-      <c r="K19" s="93">
-        <v>1</v>
       </c>
       <c r="L19" s="94">
         <v>0</v>
@@ -7805,465 +7849,454 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="94">
+        <v>0</v>
+      </c>
+      <c r="D20" s="94">
+        <v>0</v>
+      </c>
+      <c r="E20" s="94">
+        <v>0</v>
+      </c>
+      <c r="F20" s="94">
+        <v>0</v>
+      </c>
+      <c r="G20" s="94">
+        <v>0</v>
+      </c>
+      <c r="H20" s="93">
+        <v>1</v>
+      </c>
+      <c r="I20" s="93">
+        <v>1</v>
+      </c>
+      <c r="J20" s="93">
+        <v>1</v>
+      </c>
+      <c r="K20" s="93">
+        <v>1</v>
+      </c>
+      <c r="L20" s="94">
+        <v>0</v>
+      </c>
+      <c r="M20" s="94">
+        <v>0</v>
+      </c>
+      <c r="N20" s="94">
+        <v>0</v>
+      </c>
+      <c r="O20" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="94">
-        <v>0</v>
-      </c>
-      <c r="D20" s="94">
-        <v>0</v>
-      </c>
-      <c r="E20" s="94">
-        <v>0</v>
-      </c>
-      <c r="F20" s="94">
-        <v>0</v>
-      </c>
-      <c r="G20" s="94">
-        <v>0</v>
-      </c>
-      <c r="H20" s="93">
-        <v>1</v>
-      </c>
-      <c r="I20" s="93">
-        <v>1</v>
-      </c>
-      <c r="J20" s="93">
-        <v>1</v>
-      </c>
-      <c r="K20" s="93">
-        <v>1</v>
-      </c>
-      <c r="L20" s="94">
-        <v>0</v>
-      </c>
-      <c r="M20" s="94">
-        <v>0</v>
-      </c>
-      <c r="N20" s="94">
-        <v>0</v>
-      </c>
-      <c r="O20" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="C21" s="94">
+        <v>0</v>
+      </c>
+      <c r="D21" s="94">
+        <v>0</v>
+      </c>
+      <c r="E21" s="94">
+        <v>0</v>
+      </c>
+      <c r="F21" s="94">
+        <v>0</v>
+      </c>
+      <c r="G21" s="94">
+        <v>0</v>
+      </c>
+      <c r="H21" s="93">
+        <v>1</v>
+      </c>
+      <c r="I21" s="93">
+        <v>1</v>
+      </c>
+      <c r="J21" s="93">
+        <v>1</v>
+      </c>
+      <c r="K21" s="93">
+        <v>1</v>
+      </c>
+      <c r="L21" s="94">
+        <v>0</v>
+      </c>
+      <c r="M21" s="94">
+        <v>0</v>
+      </c>
+      <c r="N21" s="94">
+        <v>0</v>
+      </c>
+      <c r="O21" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="94">
-        <v>0</v>
-      </c>
-      <c r="D21" s="94">
-        <v>0</v>
-      </c>
-      <c r="E21" s="94">
-        <v>0</v>
-      </c>
-      <c r="F21" s="94">
-        <v>0</v>
-      </c>
-      <c r="G21" s="94">
-        <v>0</v>
-      </c>
-      <c r="H21" s="93">
+      <c r="C22" s="94">
+        <v>0</v>
+      </c>
+      <c r="D22" s="94">
+        <v>0</v>
+      </c>
+      <c r="E22" s="94">
+        <v>0</v>
+      </c>
+      <c r="F22" s="94">
+        <v>0</v>
+      </c>
+      <c r="G22" s="94">
+        <v>0</v>
+      </c>
+      <c r="H22" s="93">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="I21" s="93">
+      <c r="I22" s="93">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="J21" s="93">
+      <c r="J22" s="93">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K21" s="93">
+      <c r="K22" s="93">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="L21" s="94">
-        <v>0</v>
-      </c>
-      <c r="M21" s="94">
-        <v>0</v>
-      </c>
-      <c r="N21" s="94">
-        <v>0</v>
-      </c>
-      <c r="O21" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="60" t="s">
+      <c r="L22" s="94">
+        <v>0</v>
+      </c>
+      <c r="M22" s="94">
+        <v>0</v>
+      </c>
+      <c r="N22" s="94">
+        <v>0</v>
+      </c>
+      <c r="O22" s="94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="33"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B24" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="94">
-        <v>0</v>
-      </c>
-      <c r="D23" s="94">
-        <v>0</v>
-      </c>
-      <c r="E23" s="94">
-        <v>0</v>
-      </c>
-      <c r="F23" s="94">
-        <v>0</v>
-      </c>
-      <c r="G23" s="94">
-        <v>0</v>
-      </c>
-      <c r="H23" s="94">
-        <v>0</v>
-      </c>
-      <c r="I23" s="94">
-        <v>0</v>
-      </c>
-      <c r="J23" s="94">
-        <v>0</v>
-      </c>
-      <c r="K23" s="94">
-        <v>0</v>
-      </c>
-      <c r="L23" s="93">
+      <c r="C24" s="94">
+        <v>0</v>
+      </c>
+      <c r="D24" s="94">
+        <v>0</v>
+      </c>
+      <c r="E24" s="94">
+        <v>0</v>
+      </c>
+      <c r="F24" s="94">
+        <v>0</v>
+      </c>
+      <c r="G24" s="94">
+        <v>0</v>
+      </c>
+      <c r="H24" s="94">
+        <v>0</v>
+      </c>
+      <c r="I24" s="94">
+        <v>0</v>
+      </c>
+      <c r="J24" s="94">
+        <v>0</v>
+      </c>
+      <c r="K24" s="94">
+        <v>0</v>
+      </c>
+      <c r="L24" s="93">
         <f>famplan_unmet_need</f>
         <v>0</v>
       </c>
-      <c r="M23" s="93">
+      <c r="M24" s="93">
         <f>famplan_unmet_need</f>
         <v>0</v>
       </c>
-      <c r="N23" s="93">
+      <c r="N24" s="93">
         <f>famplan_unmet_need</f>
         <v>0</v>
       </c>
-      <c r="O23" s="93">
+      <c r="O24" s="93">
         <f>famplan_unmet_need</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="61" t="s">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="94">
-        <v>0</v>
-      </c>
-      <c r="D24" s="94">
-        <v>0</v>
-      </c>
-      <c r="E24" s="94">
-        <v>0</v>
-      </c>
-      <c r="F24" s="94">
-        <v>0</v>
-      </c>
-      <c r="G24" s="94">
-        <v>0</v>
-      </c>
-      <c r="H24" s="94">
-        <v>0</v>
-      </c>
-      <c r="I24" s="94">
-        <v>0</v>
-      </c>
-      <c r="J24" s="94">
-        <v>0</v>
-      </c>
-      <c r="K24" s="94">
-        <v>0</v>
-      </c>
-      <c r="L24" s="93">
+      <c r="C25" s="94">
+        <v>0</v>
+      </c>
+      <c r="D25" s="94">
+        <v>0</v>
+      </c>
+      <c r="E25" s="94">
+        <v>0</v>
+      </c>
+      <c r="F25" s="94">
+        <v>0</v>
+      </c>
+      <c r="G25" s="94">
+        <v>0</v>
+      </c>
+      <c r="H25" s="94">
+        <v>0</v>
+      </c>
+      <c r="I25" s="94">
+        <v>0</v>
+      </c>
+      <c r="J25" s="94">
+        <v>0</v>
+      </c>
+      <c r="K25" s="94">
+        <v>0</v>
+      </c>
+      <c r="L25" s="93">
         <f>(1-food_insecure)*(0.49)*(1-school_attendance) + food_insecure*(0.7)*(1-school_attendance)</f>
         <v>0.49</v>
       </c>
-      <c r="M24" s="93">
+      <c r="M25" s="93">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.49</v>
       </c>
-      <c r="N24" s="93">
+      <c r="N25" s="93">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.49</v>
       </c>
-      <c r="O24" s="93">
+      <c r="O25" s="93">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.49</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="61" t="s">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="C25" s="94">
-        <v>0</v>
-      </c>
-      <c r="D25" s="94">
-        <v>0</v>
-      </c>
-      <c r="E25" s="94">
-        <v>0</v>
-      </c>
-      <c r="F25" s="94">
-        <v>0</v>
-      </c>
-      <c r="G25" s="94">
-        <v>0</v>
-      </c>
-      <c r="H25" s="94">
-        <v>0</v>
-      </c>
-      <c r="I25" s="94">
-        <v>0</v>
-      </c>
-      <c r="J25" s="94">
-        <v>0</v>
-      </c>
-      <c r="K25" s="94">
-        <v>0</v>
-      </c>
-      <c r="L25" s="93">
+      <c r="C26" s="94">
+        <v>0</v>
+      </c>
+      <c r="D26" s="94">
+        <v>0</v>
+      </c>
+      <c r="E26" s="94">
+        <v>0</v>
+      </c>
+      <c r="F26" s="94">
+        <v>0</v>
+      </c>
+      <c r="G26" s="94">
+        <v>0</v>
+      </c>
+      <c r="H26" s="94">
+        <v>0</v>
+      </c>
+      <c r="I26" s="94">
+        <v>0</v>
+      </c>
+      <c r="J26" s="94">
+        <v>0</v>
+      </c>
+      <c r="K26" s="94">
+        <v>0</v>
+      </c>
+      <c r="L26" s="93">
         <f>(1-food_insecure)*(0.21)*(1-school_attendance) + food_insecure*(0.3)*(1-school_attendance)</f>
         <v>0.21</v>
       </c>
-      <c r="M25" s="93">
+      <c r="M26" s="93">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.21</v>
       </c>
-      <c r="N25" s="93">
+      <c r="N26" s="93">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.21</v>
       </c>
-      <c r="O25" s="93">
+      <c r="O26" s="93">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.21</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="61" t="s">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="94">
-        <v>0</v>
-      </c>
-      <c r="D26" s="94">
-        <v>0</v>
-      </c>
-      <c r="E26" s="94">
-        <v>0</v>
-      </c>
-      <c r="F26" s="94">
-        <v>0</v>
-      </c>
-      <c r="G26" s="94">
-        <v>0</v>
-      </c>
-      <c r="H26" s="94">
-        <v>0</v>
-      </c>
-      <c r="I26" s="94">
-        <v>0</v>
-      </c>
-      <c r="J26" s="94">
-        <v>0</v>
-      </c>
-      <c r="K26" s="94">
-        <v>0</v>
-      </c>
-      <c r="L26" s="93">
+      <c r="C27" s="94">
+        <v>0</v>
+      </c>
+      <c r="D27" s="94">
+        <v>0</v>
+      </c>
+      <c r="E27" s="94">
+        <v>0</v>
+      </c>
+      <c r="F27" s="94">
+        <v>0</v>
+      </c>
+      <c r="G27" s="94">
+        <v>0</v>
+      </c>
+      <c r="H27" s="94">
+        <v>0</v>
+      </c>
+      <c r="I27" s="94">
+        <v>0</v>
+      </c>
+      <c r="J27" s="94">
+        <v>0</v>
+      </c>
+      <c r="K27" s="94">
+        <v>0</v>
+      </c>
+      <c r="L27" s="93">
         <f>(1-food_insecure)*(0.3)*(1-school_attendance)</f>
         <v>0.3</v>
       </c>
-      <c r="M26" s="93">
+      <c r="M27" s="93">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.3</v>
       </c>
-      <c r="N26" s="93">
+      <c r="N27" s="93">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.3</v>
       </c>
-      <c r="O26" s="93">
+      <c r="O27" s="93">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="61" t="s">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="94">
-        <v>0</v>
-      </c>
-      <c r="D27" s="94">
-        <v>0</v>
-      </c>
-      <c r="E27" s="94">
-        <v>0</v>
-      </c>
-      <c r="F27" s="94">
-        <v>0</v>
-      </c>
-      <c r="G27" s="94">
-        <v>0</v>
-      </c>
-      <c r="H27" s="94">
-        <v>0</v>
-      </c>
-      <c r="I27" s="94">
-        <v>0</v>
-      </c>
-      <c r="J27" s="94">
-        <v>0</v>
-      </c>
-      <c r="K27" s="94">
-        <v>0</v>
-      </c>
-      <c r="L27" s="93">
+      <c r="C28" s="94">
+        <v>0</v>
+      </c>
+      <c r="D28" s="94">
+        <v>0</v>
+      </c>
+      <c r="E28" s="94">
+        <v>0</v>
+      </c>
+      <c r="F28" s="94">
+        <v>0</v>
+      </c>
+      <c r="G28" s="94">
+        <v>0</v>
+      </c>
+      <c r="H28" s="94">
+        <v>0</v>
+      </c>
+      <c r="I28" s="94">
+        <v>0</v>
+      </c>
+      <c r="J28" s="94">
+        <v>0</v>
+      </c>
+      <c r="K28" s="94">
+        <v>0</v>
+      </c>
+      <c r="L28" s="93">
         <f>(1-food_insecure)*1*school_attendance + food_insecure*1*school_attendance</f>
         <v>0</v>
       </c>
-      <c r="M27" s="93">
-        <v>0</v>
-      </c>
-      <c r="N27" s="93">
-        <v>0</v>
-      </c>
-      <c r="O27" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="M28" s="93">
+        <v>0</v>
+      </c>
+      <c r="N28" s="93">
+        <v>0</v>
+      </c>
+      <c r="O28" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="93">
-        <v>0</v>
-      </c>
-      <c r="D29" s="93">
-        <v>0</v>
-      </c>
-      <c r="E29" s="93">
-        <f t="shared" ref="E29:O29" si="0">frac_maize</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="93">
+      <c r="C30" s="93">
+        <v>0</v>
+      </c>
+      <c r="D30" s="93">
+        <v>0</v>
+      </c>
+      <c r="E30" s="93">
+        <f t="shared" ref="E30:O30" si="0">frac_maize</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="93">
+      <c r="G30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="93">
+      <c r="H30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="93">
+      <c r="I30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="93">
+      <c r="J30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="93">
+      <c r="K30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L29" s="93">
+      <c r="L30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M29" s="93">
+      <c r="M30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N29" s="93">
+      <c r="N30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O29" s="93">
+      <c r="O30" s="93">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="93">
-        <v>0</v>
-      </c>
-      <c r="D30" s="93">
-        <v>0</v>
-      </c>
-      <c r="E30" s="93">
-        <f t="shared" ref="E30:O30" si="1">frac_rice</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="93">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="93">
         <v>0</v>
@@ -8272,53 +8305,53 @@
         <v>0</v>
       </c>
       <c r="E31" s="93">
-        <f t="shared" ref="E31:O31" si="2">frac_wheat</f>
+        <f t="shared" ref="E31:O31" si="1">frac_rice</f>
         <v>0</v>
       </c>
       <c r="F31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O31" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C32" s="93">
         <v>0</v>
@@ -8327,188 +8360,199 @@
         <v>0</v>
       </c>
       <c r="E32" s="93">
-        <v>1</v>
+        <f t="shared" ref="E32:O32" si="2">frac_wheat</f>
+        <v>0</v>
       </c>
       <c r="F32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="G32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="H32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="I32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="K32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="L32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="O32" s="93">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="93">
+        <v>0</v>
+      </c>
+      <c r="D33" s="93">
+        <v>0</v>
+      </c>
+      <c r="E33" s="93">
+        <v>1</v>
+      </c>
+      <c r="F33" s="93">
+        <v>1</v>
+      </c>
+      <c r="G33" s="93">
+        <v>1</v>
+      </c>
+      <c r="H33" s="93">
+        <v>1</v>
+      </c>
+      <c r="I33" s="93">
+        <v>1</v>
+      </c>
+      <c r="J33" s="93">
+        <v>1</v>
+      </c>
+      <c r="K33" s="93">
+        <v>1</v>
+      </c>
+      <c r="L33" s="93">
+        <v>1</v>
+      </c>
+      <c r="M33" s="93">
+        <v>1</v>
+      </c>
+      <c r="N33" s="93">
+        <v>1</v>
+      </c>
+      <c r="O33" s="93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="93">
-        <f t="shared" ref="C33:O33" si="3">frac_malaria_risk</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="93">
+      <c r="C34" s="93">
+        <f t="shared" ref="C34:O34" si="3">frac_malaria_risk</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E33" s="93">
+      <c r="E34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F33" s="93">
+      <c r="F34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G33" s="93">
+      <c r="G34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H33" s="93">
+      <c r="H34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I33" s="93">
+      <c r="I34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J33" s="93">
+      <c r="J34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K33" s="93">
+      <c r="K34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L33" s="93">
+      <c r="L34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M33" s="93">
+      <c r="M34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N33" s="93">
+      <c r="N34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O33" s="93">
+      <c r="O34" s="93">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="s">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="93">
-        <v>1</v>
-      </c>
-      <c r="D34" s="93">
-        <v>1</v>
-      </c>
-      <c r="E34" s="93">
-        <v>1</v>
-      </c>
-      <c r="F34" s="93">
-        <v>1</v>
-      </c>
-      <c r="G34" s="93">
-        <v>1</v>
-      </c>
-      <c r="H34" s="93">
-        <v>1</v>
-      </c>
-      <c r="I34" s="93">
-        <v>1</v>
-      </c>
-      <c r="J34" s="93">
-        <v>1</v>
-      </c>
-      <c r="K34" s="93">
-        <v>1</v>
-      </c>
-      <c r="L34" s="93">
-        <v>1</v>
-      </c>
-      <c r="M34" s="93">
-        <v>1</v>
-      </c>
-      <c r="N34" s="93">
-        <v>1</v>
-      </c>
-      <c r="O34" s="93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="33" t="s">
+      <c r="C35" s="93">
+        <v>1</v>
+      </c>
+      <c r="D35" s="93">
+        <v>1</v>
+      </c>
+      <c r="E35" s="93">
+        <v>1</v>
+      </c>
+      <c r="F35" s="93">
+        <v>1</v>
+      </c>
+      <c r="G35" s="93">
+        <v>1</v>
+      </c>
+      <c r="H35" s="93">
+        <v>1</v>
+      </c>
+      <c r="I35" s="93">
+        <v>1</v>
+      </c>
+      <c r="J35" s="93">
+        <v>1</v>
+      </c>
+      <c r="K35" s="93">
+        <v>1</v>
+      </c>
+      <c r="L35" s="93">
+        <v>1</v>
+      </c>
+      <c r="M35" s="93">
+        <v>1</v>
+      </c>
+      <c r="N35" s="93">
+        <v>1</v>
+      </c>
+      <c r="O35" s="93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="33" t="s">
         <v>82</v>
-      </c>
-      <c r="C35" s="93">
-        <v>1</v>
-      </c>
-      <c r="D35" s="93">
-        <v>1</v>
-      </c>
-      <c r="E35" s="93">
-        <v>1</v>
-      </c>
-      <c r="F35" s="93">
-        <v>1</v>
-      </c>
-      <c r="G35" s="93">
-        <v>1</v>
-      </c>
-      <c r="H35" s="93">
-        <v>1</v>
-      </c>
-      <c r="I35" s="93">
-        <v>1</v>
-      </c>
-      <c r="J35" s="93">
-        <v>1</v>
-      </c>
-      <c r="K35" s="93">
-        <v>1</v>
-      </c>
-      <c r="L35" s="93">
-        <v>1</v>
-      </c>
-      <c r="M35" s="93">
-        <v>1</v>
-      </c>
-      <c r="N35" s="93">
-        <v>1</v>
-      </c>
-      <c r="O35" s="93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="C36" s="93">
         <v>1</v>
@@ -8552,7 +8596,7 @@
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C37" s="93">
         <v>1</v>
@@ -8596,55 +8640,99 @@
     </row>
     <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="93">
+        <v>1</v>
+      </c>
+      <c r="D38" s="93">
+        <v>1</v>
+      </c>
+      <c r="E38" s="93">
+        <v>1</v>
+      </c>
+      <c r="F38" s="93">
+        <v>1</v>
+      </c>
+      <c r="G38" s="93">
+        <v>1</v>
+      </c>
+      <c r="H38" s="93">
+        <v>1</v>
+      </c>
+      <c r="I38" s="93">
+        <v>1</v>
+      </c>
+      <c r="J38" s="93">
+        <v>1</v>
+      </c>
+      <c r="K38" s="93">
+        <v>1</v>
+      </c>
+      <c r="L38" s="93">
+        <v>1</v>
+      </c>
+      <c r="M38" s="93">
+        <v>1</v>
+      </c>
+      <c r="N38" s="93">
+        <v>1</v>
+      </c>
+      <c r="O38" s="93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="93">
-        <v>1</v>
-      </c>
-      <c r="D38" s="93">
-        <v>1</v>
-      </c>
-      <c r="E38" s="93">
-        <v>1</v>
-      </c>
-      <c r="F38" s="93">
-        <v>1</v>
-      </c>
-      <c r="G38" s="93">
-        <v>1</v>
-      </c>
-      <c r="H38" s="93">
-        <v>1</v>
-      </c>
-      <c r="I38" s="93">
-        <v>1</v>
-      </c>
-      <c r="J38" s="93">
-        <v>1</v>
-      </c>
-      <c r="K38" s="93">
-        <v>1</v>
-      </c>
-      <c r="L38" s="93">
-        <v>1</v>
-      </c>
-      <c r="M38" s="93">
-        <v>1</v>
-      </c>
-      <c r="N38" s="93">
-        <v>1</v>
-      </c>
-      <c r="O38" s="93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="33"/>
+      <c r="C39" s="93">
+        <v>1</v>
+      </c>
+      <c r="D39" s="93">
+        <v>1</v>
+      </c>
+      <c r="E39" s="93">
+        <v>1</v>
+      </c>
+      <c r="F39" s="93">
+        <v>1</v>
+      </c>
+      <c r="G39" s="93">
+        <v>1</v>
+      </c>
+      <c r="H39" s="93">
+        <v>1</v>
+      </c>
+      <c r="I39" s="93">
+        <v>1</v>
+      </c>
+      <c r="J39" s="93">
+        <v>1</v>
+      </c>
+      <c r="K39" s="93">
+        <v>1</v>
+      </c>
+      <c r="L39" s="93">
+        <v>1</v>
+      </c>
+      <c r="M39" s="93">
+        <v>1</v>
+      </c>
+      <c r="N39" s="93">
+        <v>1</v>
+      </c>
+      <c r="O39" s="93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6oMNPZOj5p1yxjZyC3cWukdFKoSh1CKATbl7uT/d1OQzf8J9XiJ/ojI28uZ+t7bQFfyXeraObfh1PN4W7pNYSw==" saltValue="6OVcnh0lkgELEvG9wcZI7g==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="B14:O21">
-    <sortCondition ref="B14:B21"/>
+  <sheetProtection selectLockedCells="1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:O22">
+    <sortCondition ref="B15:B22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8652,14 +8740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9211,13 +9299,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="53" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="C13" s="96">
         <v>0</v>
       </c>
       <c r="D13" s="96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="96">
         <v>1</v>
@@ -9255,13 +9343,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="53" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="C14" s="96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="96">
         <v>1</v>
@@ -9299,159 +9387,159 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="96">
+        <v>1</v>
+      </c>
+      <c r="D15" s="96">
+        <v>1</v>
+      </c>
+      <c r="E15" s="96">
+        <v>1</v>
+      </c>
+      <c r="F15" s="96">
+        <v>1</v>
+      </c>
+      <c r="G15" s="96">
+        <v>1</v>
+      </c>
+      <c r="H15" s="96">
+        <v>0</v>
+      </c>
+      <c r="I15" s="96">
+        <v>0</v>
+      </c>
+      <c r="J15" s="96">
+        <v>0</v>
+      </c>
+      <c r="K15" s="96">
+        <v>0</v>
+      </c>
+      <c r="L15" s="96">
+        <v>0</v>
+      </c>
+      <c r="M15" s="96">
+        <v>0</v>
+      </c>
+      <c r="N15" s="96">
+        <v>0</v>
+      </c>
+      <c r="O15" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="96">
-        <v>0</v>
-      </c>
-      <c r="D15" s="96">
-        <v>0</v>
-      </c>
-      <c r="E15" s="96">
-        <v>1</v>
-      </c>
-      <c r="F15" s="96">
-        <v>1</v>
-      </c>
-      <c r="G15" s="96">
-        <v>1</v>
-      </c>
-      <c r="H15" s="96">
-        <v>0</v>
-      </c>
-      <c r="I15" s="96">
-        <v>0</v>
-      </c>
-      <c r="J15" s="96">
-        <v>0</v>
-      </c>
-      <c r="K15" s="96">
-        <v>0</v>
-      </c>
-      <c r="L15" s="96">
-        <v>0</v>
-      </c>
-      <c r="M15" s="96">
-        <v>0</v>
-      </c>
-      <c r="N15" s="96">
-        <v>0</v>
-      </c>
-      <c r="O15" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="53"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="97"/>
-      <c r="O16" s="97"/>
+      <c r="C16" s="96">
+        <v>0</v>
+      </c>
+      <c r="D16" s="96">
+        <v>0</v>
+      </c>
+      <c r="E16" s="96">
+        <v>1</v>
+      </c>
+      <c r="F16" s="96">
+        <v>1</v>
+      </c>
+      <c r="G16" s="96">
+        <v>1</v>
+      </c>
+      <c r="H16" s="96">
+        <v>0</v>
+      </c>
+      <c r="I16" s="96">
+        <v>0</v>
+      </c>
+      <c r="J16" s="96">
+        <v>0</v>
+      </c>
+      <c r="K16" s="96">
+        <v>0</v>
+      </c>
+      <c r="L16" s="96">
+        <v>0</v>
+      </c>
+      <c r="M16" s="96">
+        <v>0</v>
+      </c>
+      <c r="N16" s="96">
+        <v>0</v>
+      </c>
+      <c r="O16" s="96">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="97"/>
+      <c r="O17" s="97"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B18" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="96">
-        <v>0</v>
-      </c>
-      <c r="D17" s="96">
-        <v>0</v>
-      </c>
-      <c r="E17" s="96">
-        <v>0</v>
-      </c>
-      <c r="F17" s="96">
-        <v>0</v>
-      </c>
-      <c r="G17" s="96">
-        <v>0</v>
-      </c>
-      <c r="H17" s="96">
-        <v>1</v>
-      </c>
-      <c r="I17" s="96">
-        <v>1</v>
-      </c>
-      <c r="J17" s="96">
-        <v>1</v>
-      </c>
-      <c r="K17" s="96">
-        <v>1</v>
-      </c>
-      <c r="L17" s="96">
-        <v>0</v>
-      </c>
-      <c r="M17" s="96">
-        <v>0</v>
-      </c>
-      <c r="N17" s="96">
-        <v>0</v>
-      </c>
-      <c r="O17" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
-      <c r="B18" s="53" t="s">
+      <c r="C18" s="96">
+        <v>0</v>
+      </c>
+      <c r="D18" s="96">
+        <v>0</v>
+      </c>
+      <c r="E18" s="96">
+        <v>0</v>
+      </c>
+      <c r="F18" s="96">
+        <v>0</v>
+      </c>
+      <c r="G18" s="96">
+        <v>0</v>
+      </c>
+      <c r="H18" s="96">
+        <v>1</v>
+      </c>
+      <c r="I18" s="96">
+        <v>1</v>
+      </c>
+      <c r="J18" s="96">
+        <v>1</v>
+      </c>
+      <c r="K18" s="96">
+        <v>1</v>
+      </c>
+      <c r="L18" s="96">
+        <v>0</v>
+      </c>
+      <c r="M18" s="96">
+        <v>0</v>
+      </c>
+      <c r="N18" s="96">
+        <v>0</v>
+      </c>
+      <c r="O18" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="57"/>
+      <c r="B19" s="53" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="96">
-        <v>0</v>
-      </c>
-      <c r="D18" s="96">
-        <v>0</v>
-      </c>
-      <c r="E18" s="96">
-        <v>0</v>
-      </c>
-      <c r="F18" s="96">
-        <v>0</v>
-      </c>
-      <c r="G18" s="96">
-        <v>0</v>
-      </c>
-      <c r="H18" s="96">
-        <v>1</v>
-      </c>
-      <c r="I18" s="96">
-        <v>1</v>
-      </c>
-      <c r="J18" s="96">
-        <v>1</v>
-      </c>
-      <c r="K18" s="96">
-        <v>1</v>
-      </c>
-      <c r="L18" s="96">
-        <v>0</v>
-      </c>
-      <c r="M18" s="96">
-        <v>0</v>
-      </c>
-      <c r="N18" s="96">
-        <v>0</v>
-      </c>
-      <c r="O18" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="98" t="s">
-        <v>189</v>
       </c>
       <c r="C19" s="96">
         <v>0</v>
@@ -9495,95 +9583,95 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="98" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="96">
+        <v>0</v>
+      </c>
+      <c r="D20" s="96">
+        <v>0</v>
+      </c>
+      <c r="E20" s="96">
+        <v>0</v>
+      </c>
+      <c r="F20" s="96">
+        <v>0</v>
+      </c>
+      <c r="G20" s="96">
+        <v>0</v>
+      </c>
+      <c r="H20" s="96">
+        <v>1</v>
+      </c>
+      <c r="I20" s="96">
+        <v>1</v>
+      </c>
+      <c r="J20" s="96">
+        <v>1</v>
+      </c>
+      <c r="K20" s="96">
+        <v>1</v>
+      </c>
+      <c r="L20" s="96">
+        <v>0</v>
+      </c>
+      <c r="M20" s="96">
+        <v>0</v>
+      </c>
+      <c r="N20" s="96">
+        <v>0</v>
+      </c>
+      <c r="O20" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="98" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="96">
-        <v>0</v>
-      </c>
-      <c r="D20" s="96">
-        <v>0</v>
-      </c>
-      <c r="E20" s="96">
-        <v>0</v>
-      </c>
-      <c r="F20" s="96">
-        <v>0</v>
-      </c>
-      <c r="G20" s="96">
-        <v>0</v>
-      </c>
-      <c r="H20" s="96">
-        <v>1</v>
-      </c>
-      <c r="I20" s="96">
-        <v>1</v>
-      </c>
-      <c r="J20" s="96">
-        <v>1</v>
-      </c>
-      <c r="K20" s="96">
-        <v>1</v>
-      </c>
-      <c r="L20" s="96">
-        <v>0</v>
-      </c>
-      <c r="M20" s="96">
-        <v>0</v>
-      </c>
-      <c r="N20" s="96">
-        <v>0</v>
-      </c>
-      <c r="O20" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="99" t="s">
+      <c r="C21" s="96">
+        <v>0</v>
+      </c>
+      <c r="D21" s="96">
+        <v>0</v>
+      </c>
+      <c r="E21" s="96">
+        <v>0</v>
+      </c>
+      <c r="F21" s="96">
+        <v>0</v>
+      </c>
+      <c r="G21" s="96">
+        <v>0</v>
+      </c>
+      <c r="H21" s="96">
+        <v>1</v>
+      </c>
+      <c r="I21" s="96">
+        <v>1</v>
+      </c>
+      <c r="J21" s="96">
+        <v>1</v>
+      </c>
+      <c r="K21" s="96">
+        <v>1</v>
+      </c>
+      <c r="L21" s="96">
+        <v>0</v>
+      </c>
+      <c r="M21" s="96">
+        <v>0</v>
+      </c>
+      <c r="N21" s="96">
+        <v>0</v>
+      </c>
+      <c r="O21" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="99" t="s">
         <v>57</v>
-      </c>
-      <c r="C21" s="96">
-        <v>0</v>
-      </c>
-      <c r="D21" s="96">
-        <v>0</v>
-      </c>
-      <c r="E21" s="96">
-        <v>0</v>
-      </c>
-      <c r="F21" s="96">
-        <v>0</v>
-      </c>
-      <c r="G21" s="96">
-        <v>0</v>
-      </c>
-      <c r="H21" s="96">
-        <v>1</v>
-      </c>
-      <c r="I21" s="96">
-        <v>1</v>
-      </c>
-      <c r="J21" s="96">
-        <v>1</v>
-      </c>
-      <c r="K21" s="96">
-        <v>1</v>
-      </c>
-      <c r="L21" s="96">
-        <v>0</v>
-      </c>
-      <c r="M21" s="96">
-        <v>0</v>
-      </c>
-      <c r="N21" s="96">
-        <v>0</v>
-      </c>
-      <c r="O21" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="53" t="s">
-        <v>88</v>
       </c>
       <c r="C22" s="96">
         <v>0</v>
@@ -9627,7 +9715,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="53" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="96">
         <v>0</v>
@@ -9671,204 +9759,204 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="96">
+        <v>0</v>
+      </c>
+      <c r="D24" s="96">
+        <v>0</v>
+      </c>
+      <c r="E24" s="96">
+        <v>0</v>
+      </c>
+      <c r="F24" s="96">
+        <v>0</v>
+      </c>
+      <c r="G24" s="96">
+        <v>0</v>
+      </c>
+      <c r="H24" s="96">
+        <v>1</v>
+      </c>
+      <c r="I24" s="96">
+        <v>1</v>
+      </c>
+      <c r="J24" s="96">
+        <v>1</v>
+      </c>
+      <c r="K24" s="96">
+        <v>1</v>
+      </c>
+      <c r="L24" s="96">
+        <v>0</v>
+      </c>
+      <c r="M24" s="96">
+        <v>0</v>
+      </c>
+      <c r="N24" s="96">
+        <v>0</v>
+      </c>
+      <c r="O24" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="96">
-        <v>0</v>
-      </c>
-      <c r="D24" s="96">
-        <v>0</v>
-      </c>
-      <c r="E24" s="96">
-        <v>0</v>
-      </c>
-      <c r="F24" s="96">
-        <v>0</v>
-      </c>
-      <c r="G24" s="96">
-        <v>0</v>
-      </c>
-      <c r="H24" s="96">
-        <v>1</v>
-      </c>
-      <c r="I24" s="96">
-        <v>1</v>
-      </c>
-      <c r="J24" s="96">
-        <v>1</v>
-      </c>
-      <c r="K24" s="96">
-        <v>1</v>
-      </c>
-      <c r="L24" s="96">
-        <v>0</v>
-      </c>
-      <c r="M24" s="96">
-        <v>0</v>
-      </c>
-      <c r="N24" s="96">
-        <v>0</v>
-      </c>
-      <c r="O24" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="53"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="97"/>
-      <c r="K25" s="97"/>
-      <c r="L25" s="97"/>
-      <c r="M25" s="97"/>
-      <c r="N25" s="97"/>
-      <c r="O25" s="97"/>
-    </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="57" t="s">
+      <c r="C25" s="96">
+        <v>0</v>
+      </c>
+      <c r="D25" s="96">
+        <v>0</v>
+      </c>
+      <c r="E25" s="96">
+        <v>0</v>
+      </c>
+      <c r="F25" s="96">
+        <v>0</v>
+      </c>
+      <c r="G25" s="96">
+        <v>0</v>
+      </c>
+      <c r="H25" s="96">
+        <v>1</v>
+      </c>
+      <c r="I25" s="96">
+        <v>1</v>
+      </c>
+      <c r="J25" s="96">
+        <v>1</v>
+      </c>
+      <c r="K25" s="96">
+        <v>1</v>
+      </c>
+      <c r="L25" s="96">
+        <v>0</v>
+      </c>
+      <c r="M25" s="96">
+        <v>0</v>
+      </c>
+      <c r="N25" s="96">
+        <v>0</v>
+      </c>
+      <c r="O25" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="53"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
+    </row>
+    <row r="27" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B27" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="96">
-        <v>0</v>
-      </c>
-      <c r="D26" s="96">
-        <v>0</v>
-      </c>
-      <c r="E26" s="96">
-        <v>0</v>
-      </c>
-      <c r="F26" s="96">
-        <v>0</v>
-      </c>
-      <c r="G26" s="96">
-        <v>0</v>
-      </c>
-      <c r="H26" s="96">
-        <v>0</v>
-      </c>
-      <c r="I26" s="96">
-        <v>0</v>
-      </c>
-      <c r="J26" s="96">
-        <v>0</v>
-      </c>
-      <c r="K26" s="96">
-        <v>0</v>
-      </c>
-      <c r="L26" s="96">
-        <v>1</v>
-      </c>
-      <c r="M26" s="96">
-        <v>0</v>
-      </c>
-      <c r="N26" s="96">
-        <v>0</v>
-      </c>
-      <c r="O26" s="96">
-        <v>0</v>
-      </c>
-      <c r="P26" s="100"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="61" t="s">
+      <c r="C27" s="96">
+        <v>0</v>
+      </c>
+      <c r="D27" s="96">
+        <v>0</v>
+      </c>
+      <c r="E27" s="96">
+        <v>0</v>
+      </c>
+      <c r="F27" s="96">
+        <v>0</v>
+      </c>
+      <c r="G27" s="96">
+        <v>0</v>
+      </c>
+      <c r="H27" s="96">
+        <v>0</v>
+      </c>
+      <c r="I27" s="96">
+        <v>0</v>
+      </c>
+      <c r="J27" s="96">
+        <v>0</v>
+      </c>
+      <c r="K27" s="96">
+        <v>0</v>
+      </c>
+      <c r="L27" s="96">
+        <v>1</v>
+      </c>
+      <c r="M27" s="96">
+        <v>0</v>
+      </c>
+      <c r="N27" s="96">
+        <v>0</v>
+      </c>
+      <c r="O27" s="96">
+        <v>0</v>
+      </c>
+      <c r="P27" s="100"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="C27" s="96">
-        <v>0</v>
-      </c>
-      <c r="D27" s="96">
-        <v>0</v>
-      </c>
-      <c r="E27" s="96">
-        <v>0</v>
-      </c>
-      <c r="F27" s="96">
-        <v>0</v>
-      </c>
-      <c r="G27" s="96">
-        <v>0</v>
-      </c>
-      <c r="H27" s="96">
-        <v>0</v>
-      </c>
-      <c r="I27" s="96">
-        <v>0</v>
-      </c>
-      <c r="J27" s="96">
-        <v>0</v>
-      </c>
-      <c r="K27" s="96">
-        <v>0</v>
-      </c>
-      <c r="L27" s="96">
-        <v>1</v>
-      </c>
-      <c r="M27" s="96">
-        <v>1</v>
-      </c>
-      <c r="N27" s="96">
-        <v>1</v>
-      </c>
-      <c r="O27" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61" t="s">
+      <c r="C28" s="96">
+        <v>0</v>
+      </c>
+      <c r="D28" s="96">
+        <v>0</v>
+      </c>
+      <c r="E28" s="96">
+        <v>0</v>
+      </c>
+      <c r="F28" s="96">
+        <v>0</v>
+      </c>
+      <c r="G28" s="96">
+        <v>0</v>
+      </c>
+      <c r="H28" s="96">
+        <v>0</v>
+      </c>
+      <c r="I28" s="96">
+        <v>0</v>
+      </c>
+      <c r="J28" s="96">
+        <v>0</v>
+      </c>
+      <c r="K28" s="96">
+        <v>0</v>
+      </c>
+      <c r="L28" s="96">
+        <v>1</v>
+      </c>
+      <c r="M28" s="96">
+        <v>1</v>
+      </c>
+      <c r="N28" s="96">
+        <v>1</v>
+      </c>
+      <c r="O28" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="57"/>
+      <c r="B29" s="61" t="s">
         <v>207</v>
-      </c>
-      <c r="C28" s="96">
-        <v>0</v>
-      </c>
-      <c r="D28" s="96">
-        <v>0</v>
-      </c>
-      <c r="E28" s="96">
-        <v>0</v>
-      </c>
-      <c r="F28" s="96">
-        <v>0</v>
-      </c>
-      <c r="G28" s="96">
-        <v>0</v>
-      </c>
-      <c r="H28" s="96">
-        <v>0</v>
-      </c>
-      <c r="I28" s="96">
-        <v>0</v>
-      </c>
-      <c r="J28" s="96">
-        <v>0</v>
-      </c>
-      <c r="K28" s="96">
-        <v>0</v>
-      </c>
-      <c r="L28" s="96">
-        <v>1</v>
-      </c>
-      <c r="M28" s="96">
-        <v>1</v>
-      </c>
-      <c r="N28" s="96">
-        <v>1</v>
-      </c>
-      <c r="O28" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="61" t="s">
-        <v>191</v>
       </c>
       <c r="C29" s="96">
         <v>0</v>
@@ -9912,114 +10000,114 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30" s="96">
+        <v>0</v>
+      </c>
+      <c r="D30" s="96">
+        <v>0</v>
+      </c>
+      <c r="E30" s="96">
+        <v>0</v>
+      </c>
+      <c r="F30" s="96">
+        <v>0</v>
+      </c>
+      <c r="G30" s="96">
+        <v>0</v>
+      </c>
+      <c r="H30" s="96">
+        <v>0</v>
+      </c>
+      <c r="I30" s="96">
+        <v>0</v>
+      </c>
+      <c r="J30" s="96">
+        <v>0</v>
+      </c>
+      <c r="K30" s="96">
+        <v>0</v>
+      </c>
+      <c r="L30" s="96">
+        <v>1</v>
+      </c>
+      <c r="M30" s="96">
+        <v>1</v>
+      </c>
+      <c r="N30" s="96">
+        <v>1</v>
+      </c>
+      <c r="O30" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="C30" s="96">
-        <v>0</v>
-      </c>
-      <c r="D30" s="96">
-        <v>0</v>
-      </c>
-      <c r="E30" s="96">
-        <v>0</v>
-      </c>
-      <c r="F30" s="96">
-        <v>0</v>
-      </c>
-      <c r="G30" s="96">
-        <v>0</v>
-      </c>
-      <c r="H30" s="96">
-        <v>0</v>
-      </c>
-      <c r="I30" s="96">
-        <v>0</v>
-      </c>
-      <c r="J30" s="96">
-        <v>0</v>
-      </c>
-      <c r="K30" s="96">
-        <v>0</v>
-      </c>
-      <c r="L30" s="96">
-        <v>1</v>
-      </c>
-      <c r="M30" s="96">
-        <v>0</v>
-      </c>
-      <c r="N30" s="96">
-        <v>0</v>
-      </c>
-      <c r="O30" s="96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="97"/>
-      <c r="K31" s="97"/>
-      <c r="L31" s="97"/>
-      <c r="M31" s="97"/>
-      <c r="N31" s="97"/>
-      <c r="O31" s="97"/>
+      <c r="C31" s="96">
+        <v>0</v>
+      </c>
+      <c r="D31" s="96">
+        <v>0</v>
+      </c>
+      <c r="E31" s="96">
+        <v>0</v>
+      </c>
+      <c r="F31" s="96">
+        <v>0</v>
+      </c>
+      <c r="G31" s="96">
+        <v>0</v>
+      </c>
+      <c r="H31" s="96">
+        <v>0</v>
+      </c>
+      <c r="I31" s="96">
+        <v>0</v>
+      </c>
+      <c r="J31" s="96">
+        <v>0</v>
+      </c>
+      <c r="K31" s="96">
+        <v>0</v>
+      </c>
+      <c r="L31" s="96">
+        <v>1</v>
+      </c>
+      <c r="M31" s="96">
+        <v>0</v>
+      </c>
+      <c r="N31" s="96">
+        <v>0</v>
+      </c>
+      <c r="O31" s="96">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="57" t="s">
+      <c r="B32" s="53"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="102"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+      <c r="N32" s="97"/>
+      <c r="O32" s="97"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B33" s="53" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" s="96">
-        <v>1</v>
-      </c>
-      <c r="D32" s="96">
-        <v>0</v>
-      </c>
-      <c r="E32" s="96">
-        <v>1</v>
-      </c>
-      <c r="F32" s="96">
-        <v>1</v>
-      </c>
-      <c r="G32" s="96">
-        <v>1</v>
-      </c>
-      <c r="H32" s="96">
-        <v>1</v>
-      </c>
-      <c r="I32" s="96">
-        <v>1</v>
-      </c>
-      <c r="J32" s="96">
-        <v>1</v>
-      </c>
-      <c r="K32" s="96">
-        <v>1</v>
-      </c>
-      <c r="L32" s="96">
-        <v>1</v>
-      </c>
-      <c r="M32" s="96">
-        <v>1</v>
-      </c>
-      <c r="N32" s="96">
-        <v>1</v>
-      </c>
-      <c r="O32" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="53" t="s">
-        <v>64</v>
       </c>
       <c r="C33" s="96">
         <v>1</v>
@@ -10063,7 +10151,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="53" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" s="96">
         <v>1</v>
@@ -10107,7 +10195,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="53" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C35" s="96">
         <v>1</v>
@@ -10151,96 +10239,96 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="96">
+        <v>1</v>
+      </c>
+      <c r="D36" s="96">
+        <v>0</v>
+      </c>
+      <c r="E36" s="96">
+        <v>1</v>
+      </c>
+      <c r="F36" s="96">
+        <v>1</v>
+      </c>
+      <c r="G36" s="96">
+        <v>1</v>
+      </c>
+      <c r="H36" s="96">
+        <v>1</v>
+      </c>
+      <c r="I36" s="96">
+        <v>1</v>
+      </c>
+      <c r="J36" s="96">
+        <v>1</v>
+      </c>
+      <c r="K36" s="96">
+        <v>1</v>
+      </c>
+      <c r="L36" s="96">
+        <v>1</v>
+      </c>
+      <c r="M36" s="96">
+        <v>1</v>
+      </c>
+      <c r="N36" s="96">
+        <v>1</v>
+      </c>
+      <c r="O36" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="96">
-        <v>1</v>
-      </c>
-      <c r="D36" s="96">
-        <v>1</v>
-      </c>
-      <c r="E36" s="96">
-        <v>1</v>
-      </c>
-      <c r="F36" s="96">
-        <v>1</v>
-      </c>
-      <c r="G36" s="96">
-        <v>1</v>
-      </c>
-      <c r="H36" s="96">
-        <v>1</v>
-      </c>
-      <c r="I36" s="96">
-        <v>1</v>
-      </c>
-      <c r="J36" s="96">
-        <v>1</v>
-      </c>
-      <c r="K36" s="96">
-        <v>1</v>
-      </c>
-      <c r="L36" s="96">
-        <v>1</v>
-      </c>
-      <c r="M36" s="96">
-        <v>1</v>
-      </c>
-      <c r="N36" s="96">
-        <v>1</v>
-      </c>
-      <c r="O36" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="103"/>
-      <c r="B37" s="53" t="s">
+      <c r="C37" s="96">
+        <v>1</v>
+      </c>
+      <c r="D37" s="96">
+        <v>1</v>
+      </c>
+      <c r="E37" s="96">
+        <v>1</v>
+      </c>
+      <c r="F37" s="96">
+        <v>1</v>
+      </c>
+      <c r="G37" s="96">
+        <v>1</v>
+      </c>
+      <c r="H37" s="96">
+        <v>1</v>
+      </c>
+      <c r="I37" s="96">
+        <v>1</v>
+      </c>
+      <c r="J37" s="96">
+        <v>1</v>
+      </c>
+      <c r="K37" s="96">
+        <v>1</v>
+      </c>
+      <c r="L37" s="96">
+        <v>1</v>
+      </c>
+      <c r="M37" s="96">
+        <v>1</v>
+      </c>
+      <c r="N37" s="96">
+        <v>1</v>
+      </c>
+      <c r="O37" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="103"/>
+      <c r="B38" s="53" t="s">
         <v>83</v>
-      </c>
-      <c r="C37" s="96">
-        <v>1</v>
-      </c>
-      <c r="D37" s="96">
-        <v>1</v>
-      </c>
-      <c r="E37" s="96">
-        <v>1</v>
-      </c>
-      <c r="F37" s="96">
-        <v>1</v>
-      </c>
-      <c r="G37" s="96">
-        <v>1</v>
-      </c>
-      <c r="H37" s="96">
-        <v>1</v>
-      </c>
-      <c r="I37" s="96">
-        <v>1</v>
-      </c>
-      <c r="J37" s="96">
-        <v>1</v>
-      </c>
-      <c r="K37" s="96">
-        <v>1</v>
-      </c>
-      <c r="L37" s="96">
-        <v>1</v>
-      </c>
-      <c r="M37" s="96">
-        <v>1</v>
-      </c>
-      <c r="N37" s="96">
-        <v>1</v>
-      </c>
-      <c r="O37" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="53" t="s">
-        <v>82</v>
       </c>
       <c r="C38" s="96">
         <v>1</v>
@@ -10284,7 +10372,7 @@
     </row>
     <row r="39" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" s="96">
         <v>1</v>
@@ -10328,107 +10416,151 @@
     </row>
     <row r="40" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="96">
+        <v>1</v>
+      </c>
+      <c r="D40" s="96">
+        <v>1</v>
+      </c>
+      <c r="E40" s="96">
+        <v>1</v>
+      </c>
+      <c r="F40" s="96">
+        <v>1</v>
+      </c>
+      <c r="G40" s="96">
+        <v>1</v>
+      </c>
+      <c r="H40" s="96">
+        <v>1</v>
+      </c>
+      <c r="I40" s="96">
+        <v>1</v>
+      </c>
+      <c r="J40" s="96">
+        <v>1</v>
+      </c>
+      <c r="K40" s="96">
+        <v>1</v>
+      </c>
+      <c r="L40" s="96">
+        <v>1</v>
+      </c>
+      <c r="M40" s="96">
+        <v>1</v>
+      </c>
+      <c r="N40" s="96">
+        <v>1</v>
+      </c>
+      <c r="O40" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="96">
-        <v>1</v>
-      </c>
-      <c r="D40" s="96">
-        <v>1</v>
-      </c>
-      <c r="E40" s="96">
-        <v>1</v>
-      </c>
-      <c r="F40" s="96">
-        <v>1</v>
-      </c>
-      <c r="G40" s="96">
-        <v>1</v>
-      </c>
-      <c r="H40" s="96">
-        <v>1</v>
-      </c>
-      <c r="I40" s="96">
-        <v>1</v>
-      </c>
-      <c r="J40" s="96">
-        <v>1</v>
-      </c>
-      <c r="K40" s="96">
-        <v>1</v>
-      </c>
-      <c r="L40" s="96">
-        <v>1</v>
-      </c>
-      <c r="M40" s="96">
-        <v>1</v>
-      </c>
-      <c r="N40" s="96">
-        <v>1</v>
-      </c>
-      <c r="O40" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="53" t="s">
+      <c r="C41" s="96">
+        <v>1</v>
+      </c>
+      <c r="D41" s="96">
+        <v>1</v>
+      </c>
+      <c r="E41" s="96">
+        <v>1</v>
+      </c>
+      <c r="F41" s="96">
+        <v>1</v>
+      </c>
+      <c r="G41" s="96">
+        <v>1</v>
+      </c>
+      <c r="H41" s="96">
+        <v>1</v>
+      </c>
+      <c r="I41" s="96">
+        <v>1</v>
+      </c>
+      <c r="J41" s="96">
+        <v>1</v>
+      </c>
+      <c r="K41" s="96">
+        <v>1</v>
+      </c>
+      <c r="L41" s="96">
+        <v>1</v>
+      </c>
+      <c r="M41" s="96">
+        <v>1</v>
+      </c>
+      <c r="N41" s="96">
+        <v>1</v>
+      </c>
+      <c r="O41" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="96">
-        <v>1</v>
-      </c>
-      <c r="D41" s="96">
-        <v>1</v>
-      </c>
-      <c r="E41" s="96">
-        <v>1</v>
-      </c>
-      <c r="F41" s="96">
-        <v>1</v>
-      </c>
-      <c r="G41" s="96">
-        <v>1</v>
-      </c>
-      <c r="H41" s="96">
-        <v>1</v>
-      </c>
-      <c r="I41" s="96">
-        <v>1</v>
-      </c>
-      <c r="J41" s="96">
-        <v>1</v>
-      </c>
-      <c r="K41" s="96">
-        <v>1</v>
-      </c>
-      <c r="L41" s="96">
-        <v>1</v>
-      </c>
-      <c r="M41" s="96">
-        <v>1</v>
-      </c>
-      <c r="N41" s="96">
-        <v>1</v>
-      </c>
-      <c r="O41" s="96">
+      <c r="C42" s="96">
+        <v>1</v>
+      </c>
+      <c r="D42" s="96">
+        <v>1</v>
+      </c>
+      <c r="E42" s="96">
+        <v>1</v>
+      </c>
+      <c r="F42" s="96">
+        <v>1</v>
+      </c>
+      <c r="G42" s="96">
+        <v>1</v>
+      </c>
+      <c r="H42" s="96">
+        <v>1</v>
+      </c>
+      <c r="I42" s="96">
+        <v>1</v>
+      </c>
+      <c r="J42" s="96">
+        <v>1</v>
+      </c>
+      <c r="K42" s="96">
+        <v>1</v>
+      </c>
+      <c r="L42" s="96">
+        <v>1</v>
+      </c>
+      <c r="M42" s="96">
+        <v>1</v>
+      </c>
+      <c r="N42" s="96">
+        <v>1</v>
+      </c>
+      <c r="O42" s="96">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UTAD6hDPFf/Ul0P2TkEmcVLwJIskng6BwO7PQn9KQppd8AxlpMXDzh2uUA/A2vdLAdLHbrkvLJZl/FHFHl0BRA==" saltValue="WyzBb18fC4LyksUq9iofgA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="R6E4Z1eMEwhWY9x8ah7fn60K/FUhiD3bjZsN+d0aneOUBQjx+MSzEQ3f4xgLromXQacg2RuQX2zps17p5X6/Gg==" saltValue="2H1gYE0Uxd3bfzXEuxrcUQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -11010,26 +11142,24 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="53" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="B31" s="96"/>
       <c r="C31" s="96"/>
       <c r="D31" s="96"/>
-      <c r="E31" s="96"/>
+      <c r="E31" s="96" t="s">
+        <v>216</v>
+      </c>
       <c r="F31" s="96"/>
-      <c r="G31" s="96" t="s">
-        <v>216</v>
-      </c>
-      <c r="H31" s="96" t="s">
-        <v>216</v>
-      </c>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
       <c r="I31" s="96"/>
       <c r="J31" s="96"/>
       <c r="K31" s="96"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B32" s="96"/>
       <c r="C32" s="96"/>
@@ -11048,7 +11178,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" s="96"/>
       <c r="C33" s="96"/>
@@ -11067,7 +11197,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="96"/>
       <c r="C34" s="96"/>
@@ -11086,7 +11216,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B35" s="96"/>
       <c r="C35" s="96"/>
@@ -11105,7 +11235,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="96"/>
       <c r="C36" s="96"/>
@@ -11124,14 +11254,16 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B37" s="96"/>
       <c r="C37" s="96"/>
       <c r="D37" s="96"/>
       <c r="E37" s="96"/>
       <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
+      <c r="G37" s="96" t="s">
+        <v>216</v>
+      </c>
       <c r="H37" s="96" t="s">
         <v>216</v>
       </c>
@@ -11141,18 +11273,14 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="96" t="s">
-        <v>216</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B38" s="96"/>
       <c r="C38" s="96"/>
       <c r="D38" s="96"/>
       <c r="E38" s="96"/>
       <c r="F38" s="96"/>
-      <c r="G38" s="96" t="s">
-        <v>216</v>
-      </c>
+      <c r="G38" s="96"/>
       <c r="H38" s="96" t="s">
         <v>216</v>
       </c>
@@ -11160,14 +11288,35 @@
       <c r="J38" s="96"/>
       <c r="K38" s="96"/>
     </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="H39" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="I39" s="96"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="96"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oiGH8ykkK4bW2BTY+0QBtgAZA6QVYaID3ACaTwjfensJoFK/mp4iBWWYi82MR3y0NDcWoVIY4HiBlMUBKqM6yA==" saltValue="6eqoI7d0CysiCWo+LkMlXw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jE1b0TVBA5pE/P7L+cdCQSfCsUOABmV4lWu9hSs+HIQ0aoN+p2CDh5bvHDw1HfKGB3mrWrP6Gq7EHXwIRs8QUw==" saltValue="G+X+bnbdBHWeDzP2p7cFoQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11541,13 +11690,13 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -12658,6 +12807,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12667,12 +12822,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12680,7 +12829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13077,7 +13226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -15980,7 +16129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -16936,7 +17085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -17246,14 +17395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17329,10 +17478,10 @@
         <v>259</v>
       </c>
       <c r="C4" s="121">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D4" s="121">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E4" s="121">
         <v>0</v>
@@ -17367,10 +17516,10 @@
         <v>259</v>
       </c>
       <c r="C6" s="121">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D6" s="121">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E6" s="121">
         <v>0</v>
@@ -17481,10 +17630,10 @@
         <v>259</v>
       </c>
       <c r="C12" s="121">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="D12" s="121">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="E12" s="121">
         <v>0</v>
@@ -17525,13 +17674,13 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -18321,14 +18470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18371,16 +18520,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="121">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E3" s="121">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="F3" s="121">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="G3" s="121">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
@@ -18389,10 +18538,10 @@
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="98" t="s">
@@ -18402,34 +18551,34 @@
         <v>1</v>
       </c>
       <c r="D5" s="121">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="121">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="F5" s="121">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="G5" s="121">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GOCV8jDgemE7dzuuRmIYljeeknnogqmqArkKarUDaviYQgtJ59RIHafgAKW2VEQf/MMJENrmBg2v2jbJ+IwMmA==" saltValue="8ZUhyEI/e1xkHczLOVME4w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P7Fljv2xXgcf52gGxiRU5lOnliCwgMAMJ6i8o5x0UxRe31wytiedBLGgitHEEiN184DDtbV3lhiQImyXgOCnZQ==" saltValue="4LtvYTWjQettQTajl384EA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="111" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18508,13 +18657,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="121">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="G3" s="121">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="H3" s="121">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -18528,13 +18677,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="121">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="G4" s="121">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="H4" s="121">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -18732,13 +18881,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G13" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H13" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -18752,13 +18901,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="121">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="G14" s="121">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="H14" s="121">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="I14" s="36"/>
     </row>
@@ -18776,13 +18925,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G15" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H15" s="121">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="I15" s="36"/>
     </row>
@@ -18797,13 +18946,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="121">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="G16" s="121">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="H16" s="121">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="I16" s="36"/>
     </row>
@@ -18839,7 +18988,7 @@
         <v>268</v>
       </c>
       <c r="D18" s="121">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E18" s="121">
         <v>0</v>
@@ -18886,7 +19035,7 @@
         <v>268</v>
       </c>
       <c r="D20" s="121">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E20" s="121">
         <v>0</v>
@@ -18932,7 +19081,7 @@
         <v>268</v>
       </c>
       <c r="D22" s="121">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E22" s="121">
         <v>0</v>
@@ -19371,19 +19520,19 @@
         <v>268</v>
       </c>
       <c r="D42" s="121">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="121">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F42" s="121">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="121">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H42" s="121">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -19391,19 +19540,19 @@
         <v>269</v>
       </c>
       <c r="D43" s="121">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="E43" s="121">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="F43" s="121">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="G43" s="121">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="H43" s="121">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -19437,19 +19586,19 @@
         <v>268</v>
       </c>
       <c r="D45" s="121">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="E45" s="121">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="F45" s="121">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="G45" s="121">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="H45" s="121">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -19483,19 +19632,19 @@
         <v>268</v>
       </c>
       <c r="D47" s="121">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E47" s="121">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="F47" s="121">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="G47" s="121">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="H47" s="121">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -19512,7 +19661,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="E48" s="121">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F48" s="121">
         <v>0</v>
@@ -19529,10 +19678,10 @@
         <v>268</v>
       </c>
       <c r="D49" s="121">
-        <v>0.51</v>
+        <v>0.88</v>
       </c>
       <c r="E49" s="121">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="F49" s="121">
         <v>0</v>
@@ -19552,14 +19701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D7" sqref="D7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19708,16 +19857,16 @@
         <v>268</v>
       </c>
       <c r="D7" s="121">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="E7" s="121">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F7" s="121">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="G7" s="121">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H7" s="142"/>
     </row>
@@ -19728,7 +19877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19763,7 +19912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -19972,7 +20121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -20305,7 +20454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -20666,7 +20815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -20771,7 +20920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -20974,7 +21123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -21215,20 +21364,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
@@ -21237,7 +21386,7 @@
       <c r="A1" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="63" t="s">
         <v>183</v>
       </c>
       <c r="C1" s="63" t="s">
@@ -21249,19 +21398,19 @@
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D2" s="81"/>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>178</v>
@@ -21272,20 +21421,20 @@
       <c r="D3" s="81"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KAK9fjAi0tB9w1PUqeUNgZBXNYGF7t08YNHBjS6f2/uFBIh1t5g5f3mTDoaIfBvsASpqT35v7SBH94ZWCC9pQg==" saltValue="GSmV5uySc7GZpAmsyAcl7Q==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A28" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21811,7 +21960,7 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="53" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="B31" s="85">
         <v>0</v>
@@ -21820,7 +21969,7 @@
         <v>0.95</v>
       </c>
       <c r="D31" s="86">
-        <v>0.35</v>
+        <v>9.36</v>
       </c>
       <c r="E31" s="86" t="s">
         <v>201</v>
@@ -21828,7 +21977,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B32" s="85">
         <v>0</v>
@@ -21837,7 +21986,7 @@
         <v>0.95</v>
       </c>
       <c r="D32" s="86">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="E32" s="86" t="s">
         <v>201</v>
@@ -21845,7 +21994,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" s="85">
         <v>0</v>
@@ -21854,7 +22003,7 @@
         <v>0.95</v>
       </c>
       <c r="D33" s="86">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="E33" s="86" t="s">
         <v>201</v>
@@ -21862,7 +22011,7 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="85">
         <v>0</v>
@@ -21871,7 +22020,7 @@
         <v>0.95</v>
       </c>
       <c r="D34" s="86">
-        <v>50.26</v>
+        <v>2.8</v>
       </c>
       <c r="E34" s="86" t="s">
         <v>201</v>
@@ -21879,7 +22028,7 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B35" s="85">
         <v>0</v>
@@ -21888,15 +22037,15 @@
         <v>0.95</v>
       </c>
       <c r="D35" s="86">
-        <v>36.1</v>
+        <v>50.26</v>
       </c>
       <c r="E35" s="86" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="85">
         <v>0</v>
@@ -21905,16 +22054,15 @@
         <v>0.95</v>
       </c>
       <c r="D36" s="86">
-        <v>231.85</v>
+        <v>36.1</v>
       </c>
       <c r="E36" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="F36" s="35"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B37" s="85">
         <v>0</v>
@@ -21923,15 +22071,16 @@
         <v>0.95</v>
       </c>
       <c r="D37" s="86">
-        <v>1.5</v>
+        <v>231.85</v>
       </c>
       <c r="E37" s="86" t="s">
         <v>201</v>
       </c>
+      <c r="F37" s="35"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B38" s="85">
         <v>0</v>
@@ -21940,31 +22089,48 @@
         <v>0.95</v>
       </c>
       <c r="D38" s="86">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E38" s="86" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F39" s="36"/>
+      <c r="A39" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="85">
+        <v>0</v>
+      </c>
+      <c r="C39" s="85">
+        <v>0.95</v>
+      </c>
+      <c r="D39" s="86">
+        <v>1</v>
+      </c>
+      <c r="E39" s="86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wtv/HM4kAqRqMIiLkAYQC7Lcjqz7qSMF7Fo+6qi+BfjtDEm3dmaJR2oG6r16A5EzV4QlJ3rsskLmp+Scq5MAEw==" saltValue="phkuzZ1elu1sMpGSD/cRFg==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="A2:D38">
-    <sortCondition ref="A2:A38"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="w1vMW0gL06Vb5eNknt9lNnNFj5i+5F/VjK9YWPtBe7dpzfitI0zN4F5rJ0KR87XA6mi0Itdi0rm/vuMY7vlK8w==" saltValue="gM9mpifVxG/optWd3F61aQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D39">
+    <sortCondition ref="A2:A39"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E38</xm:sqref>
+          <xm:sqref>E2:E39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>